<commit_message>
AUD first working version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_Market.xlsx
@@ -3004,94 +3004,94 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 09:22:05</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{534982F6-9A1D-4A33-AF4F-24B22E23CE2E}</stp>
+        <stp>{09939762-717F-4E52-8CA9-E01C5A190F44}</stp>
+        <tr r="Q5" s="64"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{15A485A5-D4A3-4BF9-B80C-46968DCFA27F}</stp>
+        <tr r="J4" s="15"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{74C01410-1083-4AA7-8982-988459EE4A5C}</stp>
+        <tr r="O4" s="22"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{82101283-110D-46E0-AA52-5C8992E5B81A}</stp>
+        <tr r="O4" s="65"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{21B68B08-9BB4-4406-AEFD-3378F608CF4D}</stp>
+        <tr r="M6" s="8"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{84AC724C-F7F8-44D7-ABD9-1CA95A8955ED}</stp>
+        <tr r="P4" s="26"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:43:55</v>
+        <stp/>
+        <stp>{ED9B07FC-64B9-44E1-B3C9-EDA1965C2BEB}</stp>
         <tr r="O5" s="18"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:12:36</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{EF4295A3-0C82-4563-B203-DA800B87B628}</stp>
-        <tr r="M6" s="8"/>
+        <stp>{8D242C0F-DE49-44FC-B7BB-5A4724F52C4E}</stp>
+        <tr r="P4" s="12"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:13:49</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{B0E7D24A-87B9-4824-A966-31BBE4098D7D}</stp>
+        <stp>{5C84809A-5C72-4B3F-97E0-1950531F3D6D}</stp>
+        <tr r="P4" s="11"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{5C95C3D6-BCDA-453A-8647-DD456780D1D0}</stp>
         <tr r="N4" s="16"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{3CDC4104-3031-42D9-AA83-65D54D56FE53}</stp>
-        <tr r="P4" s="12"/>
+        <stp>{70814F26-090B-4581-9718-A944317E20FB}</stp>
+        <tr r="M6" s="7"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:12:36</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{56D88654-7792-4A3C-B9A6-8A31E801DFC2}</stp>
+        <stp>{D9C2CEA5-9B24-4A1E-BB72-9E478F22C49D}</stp>
+        <tr r="P4" s="25"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{BF659609-C77B-4E32-B82F-0163199DC53E}</stp>
+        <tr r="K5" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:39:37</v>
+        <stp/>
+        <stp>{318D5ACC-3EED-4C21-B8DC-7718BE198A6F}</stp>
         <tr r="O5" s="17"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
         <stp/>
-        <stp>{97F50E87-E0B0-45C2-833C-F99E5598352B}</stp>
-        <tr r="Q5" s="64"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:37</v>
-        <stp/>
-        <stp>{3825F087-3EFE-495F-A41B-EEDBBEA83842}</stp>
-        <tr r="P4" s="26"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:37</v>
-        <stp/>
-        <stp>{6CA0902C-D22D-4404-B96A-0695AA324A07}</stp>
-        <tr r="K5" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:37</v>
-        <stp/>
-        <stp>{1F6E3E7D-DB5A-443A-991B-05DB8A1D0727}</stp>
-        <tr r="P4" s="25"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:38</v>
-        <stp/>
-        <stp>{868E78B6-88BF-4EF8-BC28-B0389D52919D}</stp>
+        <stp>{4D291D04-57B0-4E5B-8F75-8F91B21421AE}</stp>
         <tr r="O4" s="23"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:21:40</v>
-        <stp/>
-        <stp>{5714431D-FFD0-4D96-AB33-E06298353416}</stp>
-        <tr r="J4" s="15"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:38</v>
-        <stp/>
-        <stp>{16DEB325-BC40-4025-8E48-0CE7B5FBDDD5}</stp>
-        <tr r="P4" s="11"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:37</v>
-        <stp/>
-        <stp>{D6A33BAA-F9C2-4958-B2EE-B97E480E900C}</stp>
-        <tr r="O4" s="22"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:36</v>
-        <stp/>
-        <stp>{144CF197-FC60-46BF-A402-487A987F2648}</stp>
-        <tr r="M6" s="7"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:12:38</v>
-        <stp/>
-        <stp>{66625AB5-BF72-4DFD-8408-335B0B4FB1C2}</stp>
-        <tr r="O4" s="65"/>
       </tp>
     </main>
   </volType>
@@ -3459,7 +3459,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="266">
-        <v>41808.383472222224</v>
+        <v>41808.610439814816</v>
       </c>
       <c r="E5" s="253"/>
       <c r="G5" s="5"/>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D7" s="263">
         <f>_xll.ohTrigger(Deposits!R3,FRA!X3,Futures3M!Z4,FuturesHWConvAdj!Q3,Swaps1M!Y3,Swap3M!Z3,Swap6M!Z3,BasisSwap1M3M!X3,BasisSwap3M6M!X3,OIS!Y3)</f>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E7" s="253"/>
       <c r="G7" s="5"/>
@@ -4287,7 +4287,7 @@
       <c r="N4" s="115"/>
       <c r="O4" s="134" t="str">
         <f>_xll.RData(O5:O18,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:12:38</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="P4" s="188" t="s">
         <v>162</v>
@@ -5393,7 +5393,7 @@
       <c r="O4" s="115"/>
       <c r="P4" s="497" t="str">
         <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="Z6" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F6,Y6/100,Trigger)</f>
-        <v>2.4999999999997247E-5</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="126"/>
       <c r="AB6" s="12"/>
@@ -5883,7 +5883,7 @@
       </c>
       <c r="Z10" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F10,Y10/100,Trigger)</f>
-        <v>1.0000000000000633E-4</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="126"/>
       <c r="AB10" s="12"/>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="Z11" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F11,Y11/100,Trigger)</f>
-        <v>2.5000000000000022E-4</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="126"/>
       <c r="AB11" s="12"/>
@@ -8574,7 +8574,7 @@
       <c r="O4" s="115"/>
       <c r="P4" s="134" t="str">
         <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="Z12" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F12,Y12/100,Trigger)</f>
-        <v>3.0000000000000165E-4</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="126"/>
       <c r="AB12" s="12"/>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="Z13" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F13,Y13/100,Trigger)</f>
-        <v>3.2499999999999196E-4</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="126"/>
       <c r="AB13" s="12"/>
@@ -9372,7 +9372,7 @@
       </c>
       <c r="Z14" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F14,Y14/100,Trigger)</f>
-        <v>3.4999999999999615E-4</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="126"/>
       <c r="AB14" s="12"/>
@@ -9449,7 +9449,7 @@
       </c>
       <c r="Z15" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F15,Y15/100,Trigger)</f>
-        <v>4.2499999999999483E-4</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="126"/>
       <c r="AB15" s="12"/>
@@ -9526,7 +9526,7 @@
       </c>
       <c r="Z16" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F16,Y16/100,Trigger)</f>
-        <v>4.4999999999999901E-4</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="126"/>
       <c r="AB16" s="12"/>
@@ -9603,7 +9603,7 @@
       </c>
       <c r="Z17" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F17,Y17/100,Trigger)</f>
-        <v>4.750000000000032E-4</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="126"/>
       <c r="AB17" s="12"/>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="Z18" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F18,Y18/100,Trigger)</f>
-        <v>5.0000000000000738E-4</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="126"/>
       <c r="AB18" s="12"/>
@@ -9834,7 +9834,7 @@
       </c>
       <c r="Z20" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20/100,Trigger)</f>
-        <v>5.2499999999999769E-4</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="126"/>
       <c r="AB20" s="12"/>
@@ -10065,7 +10065,7 @@
       </c>
       <c r="Z23" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F23,Y23/100,Trigger)</f>
-        <v>5.4999999999999494E-4</v>
+        <v>0</v>
       </c>
       <c r="AA23" s="126"/>
       <c r="AB23" s="12"/>
@@ -10450,7 +10450,7 @@
       </c>
       <c r="Z28" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F28,Y28/100,Trigger)</f>
-        <v>5.0000000000000738E-4</v>
+        <v>0</v>
       </c>
       <c r="AA28" s="126"/>
       <c r="AB28" s="12"/>
@@ -10835,7 +10835,7 @@
       </c>
       <c r="Z33" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F33,Y33/100,Trigger)</f>
-        <v>5.0000000000000738E-4</v>
+        <v>0</v>
       </c>
       <c r="AA33" s="126"/>
       <c r="AB33" s="12"/>
@@ -11220,7 +11220,7 @@
       </c>
       <c r="Z38" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F38,Y38/100,Trigger)</f>
-        <v>5.0000000000000044E-4</v>
+        <v>0</v>
       </c>
       <c r="AA38" s="126"/>
       <c r="AB38" s="12"/>
@@ -11374,7 +11374,7 @@
       </c>
       <c r="Z40" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F40,Y40/100,Trigger)</f>
-        <v>5.0000000000000044E-4</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="126"/>
       <c r="AB40" s="12"/>
@@ -11730,7 +11730,7 @@
       <c r="O4" s="115"/>
       <c r="P4" s="134" t="str">
         <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:12:38</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -11890,7 +11890,7 @@
       </c>
       <c r="X6" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/10000,Trigger)</f>
-        <v>2.5000000000000066E-5</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="126"/>
       <c r="Z6" s="12"/>
@@ -12168,7 +12168,7 @@
       </c>
       <c r="X10" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/10000,Trigger)</f>
-        <v>2.4999999999999957E-5</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="126"/>
     </row>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="X11" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/10000,Trigger)</f>
-        <v>1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="126"/>
     </row>
@@ -12302,7 +12302,7 @@
       </c>
       <c r="X12" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>1.2499999999999924E-5</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="126"/>
     </row>
@@ -12369,7 +12369,7 @@
       </c>
       <c r="X13" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/10000,Trigger)</f>
-        <v>1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="126"/>
     </row>
@@ -14521,7 +14521,7 @@
       <c r="O4" s="115"/>
       <c r="P4" s="134" t="str">
         <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -15111,7 +15111,7 @@
       </c>
       <c r="X12" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>-1.2499999999999924E-5</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="126"/>
       <c r="Z12" s="12"/>
@@ -15324,7 +15324,7 @@
       </c>
       <c r="X15" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="126"/>
       <c r="Z15" s="12"/>
@@ -15537,7 +15537,7 @@
       </c>
       <c r="X18" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F18,W18/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="126"/>
       <c r="Z18" s="12"/>
@@ -15892,7 +15892,7 @@
       </c>
       <c r="X23" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F23,W23/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="126"/>
       <c r="Z23" s="12"/>
@@ -17464,7 +17464,7 @@
       <c r="J5" s="393"/>
       <c r="K5" s="369" t="str">
         <f>_xll.RData(K6:K12,L5:M5,"RTFEED:IDN",,,L6)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="L5" s="370" t="s">
         <v>227</v>
@@ -17580,7 +17580,7 @@
       </c>
       <c r="H7" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E7)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I7" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -17647,7 +17647,7 @@
       </c>
       <c r="H8" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E8)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I8" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -17714,7 +17714,7 @@
       </c>
       <c r="H9" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E9)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I9" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -17781,7 +17781,7 @@
       </c>
       <c r="H10" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E10)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I10" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -17848,7 +17848,7 @@
       </c>
       <c r="H11" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E11)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I11" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -17915,7 +17915,7 @@
       </c>
       <c r="H12" s="367" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v>qlLibor - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="I12" s="367" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -18237,7 +18237,7 @@
       </c>
       <c r="M6" s="310" t="str">
         <f>_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
-        <v>Updated at 09:12:36</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="N6" s="310" t="s">
         <v>227</v>
@@ -18288,7 +18288,7 @@
       </c>
       <c r="G7" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F7)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H7" s="21"/>
       <c r="J7" s="270"/>
@@ -18359,7 +18359,7 @@
       </c>
       <c r="G8" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F8)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H8" s="21"/>
       <c r="J8" s="270"/>
@@ -18430,7 +18430,7 @@
       </c>
       <c r="G9" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F9)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H9" s="21"/>
       <c r="J9" s="270"/>
@@ -18501,7 +18501,7 @@
       </c>
       <c r="G10" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F10)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H10" s="21"/>
       <c r="J10" s="270"/>
@@ -18572,7 +18572,7 @@
       </c>
       <c r="G11" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F11)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="270"/>
@@ -18643,7 +18643,7 @@
       </c>
       <c r="G12" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F12)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H12" s="21"/>
       <c r="J12" s="270"/>
@@ -18714,7 +18714,7 @@
       </c>
       <c r="G13" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F13)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H13" s="21"/>
       <c r="J13" s="270"/>
@@ -18785,7 +18785,7 @@
       </c>
       <c r="G14" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F14)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H14" s="21"/>
       <c r="J14" s="270"/>
@@ -18856,7 +18856,7 @@
       </c>
       <c r="G15" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F15)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="270"/>
@@ -18927,7 +18927,7 @@
       </c>
       <c r="G16" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F16)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H16" s="21"/>
       <c r="J16" s="270"/>
@@ -18998,7 +18998,7 @@
       </c>
       <c r="G17" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F17)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H17" s="21"/>
       <c r="J17" s="270"/>
@@ -19069,7 +19069,7 @@
       </c>
       <c r="G18" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F18)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H18" s="21"/>
       <c r="J18" s="270"/>
@@ -19140,7 +19140,7 @@
       </c>
       <c r="G19" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F19)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H19" s="21"/>
       <c r="J19" s="270"/>
@@ -19211,7 +19211,7 @@
       </c>
       <c r="G20" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F20)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H20" s="21"/>
       <c r="J20" s="270"/>
@@ -19282,7 +19282,7 @@
       </c>
       <c r="G21" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F21)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H21" s="21"/>
       <c r="J21" s="270"/>
@@ -19353,7 +19353,7 @@
       </c>
       <c r="G22" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F22)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H22" s="21"/>
       <c r="J22" s="270"/>
@@ -19391,7 +19391,7 @@
       </c>
       <c r="G23" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F23)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H23" s="21"/>
       <c r="J23" s="270"/>
@@ -19429,7 +19429,7 @@
       </c>
       <c r="G24" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F24)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H24" s="21"/>
       <c r="J24" s="270"/>
@@ -19473,7 +19473,7 @@
       </c>
       <c r="G25" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F25)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H25" s="21"/>
       <c r="J25" s="270"/>
@@ -19517,7 +19517,7 @@
       </c>
       <c r="G26" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F26)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H26" s="21"/>
       <c r="J26" s="270"/>
@@ -19561,7 +19561,7 @@
       </c>
       <c r="G27" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F27)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H27" s="21"/>
       <c r="J27" s="270"/>
@@ -19605,7 +19605,7 @@
       </c>
       <c r="G28" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F28)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H28" s="21"/>
       <c r="J28" s="270"/>
@@ -19649,7 +19649,7 @@
       </c>
       <c r="G29" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F29)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H29" s="21"/>
       <c r="J29" s="270"/>
@@ -19693,7 +19693,7 @@
       </c>
       <c r="G30" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F30)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H30" s="21"/>
       <c r="J30" s="270"/>
@@ -19737,7 +19737,7 @@
       </c>
       <c r="G31" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F31)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H31" s="21"/>
     </row>
@@ -19759,7 +19759,7 @@
       </c>
       <c r="G32" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F32)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H32" s="21"/>
     </row>
@@ -19781,7 +19781,7 @@
       </c>
       <c r="G33" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F33)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H33" s="21"/>
     </row>
@@ -19803,7 +19803,7 @@
       </c>
       <c r="G34" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F34)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H34" s="21"/>
     </row>
@@ -19825,7 +19825,7 @@
       </c>
       <c r="G35" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F35)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H35" s="21"/>
     </row>
@@ -19847,7 +19847,7 @@
       </c>
       <c r="G36" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F36)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H36" s="21"/>
     </row>
@@ -19869,7 +19869,7 @@
       </c>
       <c r="G37" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F37)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H37" s="21"/>
     </row>
@@ -19891,7 +19891,7 @@
       </c>
       <c r="G38" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F38)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H38" s="21"/>
     </row>
@@ -19913,7 +19913,7 @@
       </c>
       <c r="G39" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F39)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H39" s="21"/>
     </row>
@@ -19935,7 +19935,7 @@
       </c>
       <c r="G40" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F40)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H40" s="21"/>
     </row>
@@ -19957,7 +19957,7 @@
       </c>
       <c r="G41" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F41)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H41" s="21"/>
     </row>
@@ -19979,7 +19979,7 @@
       </c>
       <c r="G42" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F42)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H42" s="21"/>
     </row>
@@ -20001,7 +20001,7 @@
       </c>
       <c r="G43" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F43)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H43" s="21"/>
     </row>
@@ -20023,7 +20023,7 @@
       </c>
       <c r="G44" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F44)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H44" s="21"/>
     </row>
@@ -20045,7 +20045,7 @@
       </c>
       <c r="G45" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F45)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H45" s="21"/>
     </row>
@@ -20067,7 +20067,7 @@
       </c>
       <c r="G46" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F46)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H46" s="21"/>
     </row>
@@ -20089,7 +20089,7 @@
       </c>
       <c r="G47" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F47)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H47" s="21"/>
     </row>
@@ -20111,7 +20111,7 @@
       </c>
       <c r="G48" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F48)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H48" s="21"/>
     </row>
@@ -20133,7 +20133,7 @@
       </c>
       <c r="G49" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F49)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H49" s="21"/>
     </row>
@@ -20155,7 +20155,7 @@
       </c>
       <c r="G50" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F50)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H50" s="21"/>
     </row>
@@ -20177,7 +20177,7 @@
       </c>
       <c r="G51" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F51)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H51" s="21"/>
     </row>
@@ -20199,7 +20199,7 @@
       </c>
       <c r="G52" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F52)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H52" s="21"/>
     </row>
@@ -20221,7 +20221,7 @@
       </c>
       <c r="G53" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F53)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H53" s="21"/>
     </row>
@@ -20243,7 +20243,7 @@
       </c>
       <c r="G54" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F54)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H54" s="21"/>
     </row>
@@ -20265,7 +20265,7 @@
       </c>
       <c r="G55" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F55)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H55" s="21"/>
     </row>
@@ -20287,7 +20287,7 @@
       </c>
       <c r="G56" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F56)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H56" s="21"/>
     </row>
@@ -20309,7 +20309,7 @@
       </c>
       <c r="G57" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F57)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H57" s="21"/>
     </row>
@@ -20331,7 +20331,7 @@
       </c>
       <c r="G58" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F58)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H58" s="21"/>
     </row>
@@ -20353,7 +20353,7 @@
       </c>
       <c r="G59" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F59)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H59" s="21"/>
     </row>
@@ -20375,7 +20375,7 @@
       </c>
       <c r="G60" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F60)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H60" s="21"/>
     </row>
@@ -20397,7 +20397,7 @@
       </c>
       <c r="G61" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F61)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H61" s="21"/>
     </row>
@@ -20419,7 +20419,7 @@
       </c>
       <c r="G62" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F62)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H62" s="21"/>
     </row>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="G63" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F63)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H63" s="21"/>
     </row>
@@ -20463,7 +20463,7 @@
       </c>
       <c r="G64" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F64)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H64" s="21"/>
     </row>
@@ -20485,7 +20485,7 @@
       </c>
       <c r="G65" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F65)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H65" s="21"/>
     </row>
@@ -20507,7 +20507,7 @@
       </c>
       <c r="G66" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F66)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H66" s="21"/>
     </row>
@@ -20784,7 +20784,7 @@
       </c>
       <c r="M6" s="310" t="str">
         <f>_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
-        <v>Updated at 09:12:36</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="N6" s="310" t="s">
         <v>227</v>
@@ -20835,7 +20835,7 @@
       </c>
       <c r="G7" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F7)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H7" s="21"/>
       <c r="J7" s="270"/>
@@ -20906,7 +20906,7 @@
       </c>
       <c r="G8" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F8)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H8" s="21"/>
       <c r="J8" s="270"/>
@@ -20977,7 +20977,7 @@
       </c>
       <c r="G9" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F9)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H9" s="21"/>
       <c r="J9" s="270"/>
@@ -21048,7 +21048,7 @@
       </c>
       <c r="G10" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F10)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H10" s="21"/>
       <c r="J10" s="270"/>
@@ -21119,7 +21119,7 @@
       </c>
       <c r="G11" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F11)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H11" s="21"/>
       <c r="J11" s="270"/>
@@ -21190,7 +21190,7 @@
       </c>
       <c r="G12" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F12)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H12" s="21"/>
       <c r="J12" s="270"/>
@@ -21261,7 +21261,7 @@
       </c>
       <c r="G13" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F13)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H13" s="21"/>
       <c r="J13" s="270"/>
@@ -21332,7 +21332,7 @@
       </c>
       <c r="G14" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F14)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H14" s="21"/>
       <c r="J14" s="270"/>
@@ -21403,7 +21403,7 @@
       </c>
       <c r="G15" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F15)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H15" s="21"/>
       <c r="J15" s="270"/>
@@ -21474,7 +21474,7 @@
       </c>
       <c r="G16" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F16)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H16" s="21"/>
       <c r="J16" s="270"/>
@@ -21545,7 +21545,7 @@
       </c>
       <c r="G17" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F17)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H17" s="21"/>
       <c r="J17" s="270"/>
@@ -21616,7 +21616,7 @@
       </c>
       <c r="G18" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F18)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H18" s="21"/>
       <c r="J18" s="270"/>
@@ -21687,7 +21687,7 @@
       </c>
       <c r="G19" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F19)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H19" s="21"/>
       <c r="J19" s="270"/>
@@ -21758,7 +21758,7 @@
       </c>
       <c r="G20" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F20)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H20" s="21"/>
       <c r="J20" s="270"/>
@@ -21829,7 +21829,7 @@
       </c>
       <c r="G21" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F21)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H21" s="21"/>
       <c r="J21" s="270"/>
@@ -21900,7 +21900,7 @@
       </c>
       <c r="G22" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F22)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H22" s="21"/>
       <c r="J22" s="270"/>
@@ -21938,7 +21938,7 @@
       </c>
       <c r="G23" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F23)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H23" s="21"/>
       <c r="J23" s="270"/>
@@ -21976,7 +21976,7 @@
       </c>
       <c r="G24" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F24)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H24" s="21"/>
       <c r="J24" s="270"/>
@@ -22020,7 +22020,7 @@
       </c>
       <c r="G25" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F25)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H25" s="21"/>
       <c r="J25" s="270"/>
@@ -22064,7 +22064,7 @@
       </c>
       <c r="G26" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F26)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H26" s="21"/>
       <c r="J26" s="270"/>
@@ -22108,7 +22108,7 @@
       </c>
       <c r="G27" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F27)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H27" s="21"/>
       <c r="J27" s="270"/>
@@ -22152,7 +22152,7 @@
       </c>
       <c r="G28" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F28)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H28" s="21"/>
       <c r="J28" s="270"/>
@@ -22196,7 +22196,7 @@
       </c>
       <c r="G29" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F29)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H29" s="21"/>
       <c r="J29" s="270"/>
@@ -22240,7 +22240,7 @@
       </c>
       <c r="G30" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F30)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H30" s="21"/>
       <c r="J30" s="270"/>
@@ -22284,7 +22284,7 @@
       </c>
       <c r="G31" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F31)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H31" s="21"/>
     </row>
@@ -22306,7 +22306,7 @@
       </c>
       <c r="G32" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F32)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H32" s="21"/>
     </row>
@@ -22328,7 +22328,7 @@
       </c>
       <c r="G33" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F33)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H33" s="21"/>
     </row>
@@ -22350,7 +22350,7 @@
       </c>
       <c r="G34" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F34)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H34" s="21"/>
     </row>
@@ -22372,7 +22372,7 @@
       </c>
       <c r="G35" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F35)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H35" s="21"/>
     </row>
@@ -22394,7 +22394,7 @@
       </c>
       <c r="G36" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F36)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H36" s="21"/>
     </row>
@@ -22416,7 +22416,7 @@
       </c>
       <c r="G37" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F37)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H37" s="21"/>
     </row>
@@ -22438,7 +22438,7 @@
       </c>
       <c r="G38" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F38)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H38" s="21"/>
     </row>
@@ -22460,7 +22460,7 @@
       </c>
       <c r="G39" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F39)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H39" s="21"/>
     </row>
@@ -22482,7 +22482,7 @@
       </c>
       <c r="G40" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F40)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H40" s="21"/>
     </row>
@@ -22504,7 +22504,7 @@
       </c>
       <c r="G41" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F41)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H41" s="21"/>
     </row>
@@ -22526,7 +22526,7 @@
       </c>
       <c r="G42" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F42)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H42" s="21"/>
     </row>
@@ -22548,7 +22548,7 @@
       </c>
       <c r="G43" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F43)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H43" s="21"/>
     </row>
@@ -22570,7 +22570,7 @@
       </c>
       <c r="G44" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F44)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H44" s="21"/>
     </row>
@@ -22592,7 +22592,7 @@
       </c>
       <c r="G45" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F45)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H45" s="21"/>
     </row>
@@ -22614,7 +22614,7 @@
       </c>
       <c r="G46" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F46)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H46" s="21"/>
     </row>
@@ -22636,7 +22636,7 @@
       </c>
       <c r="G47" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F47)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H47" s="21"/>
     </row>
@@ -22658,7 +22658,7 @@
       </c>
       <c r="G48" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F48)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H48" s="21"/>
     </row>
@@ -22680,7 +22680,7 @@
       </c>
       <c r="G49" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F49)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H49" s="21"/>
     </row>
@@ -22702,7 +22702,7 @@
       </c>
       <c r="G50" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F50)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H50" s="21"/>
     </row>
@@ -22724,7 +22724,7 @@
       </c>
       <c r="G51" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F51)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H51" s="21"/>
     </row>
@@ -22746,7 +22746,7 @@
       </c>
       <c r="G52" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F52)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H52" s="21"/>
     </row>
@@ -22768,7 +22768,7 @@
       </c>
       <c r="G53" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F53)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H53" s="21"/>
     </row>
@@ -22790,7 +22790,7 @@
       </c>
       <c r="G54" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F54)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H54" s="21"/>
     </row>
@@ -22812,7 +22812,7 @@
       </c>
       <c r="G55" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F55)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H55" s="21"/>
     </row>
@@ -22834,7 +22834,7 @@
       </c>
       <c r="G56" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F56)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H56" s="21"/>
     </row>
@@ -22856,7 +22856,7 @@
       </c>
       <c r="G57" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F57)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H57" s="21"/>
     </row>
@@ -22878,7 +22878,7 @@
       </c>
       <c r="G58" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F58)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H58" s="21"/>
     </row>
@@ -22900,7 +22900,7 @@
       </c>
       <c r="G59" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F59)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H59" s="21"/>
     </row>
@@ -22922,7 +22922,7 @@
       </c>
       <c r="G60" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F60)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H60" s="21"/>
     </row>
@@ -22944,7 +22944,7 @@
       </c>
       <c r="G61" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F61)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H61" s="21"/>
     </row>
@@ -22966,7 +22966,7 @@
       </c>
       <c r="G62" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F62)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H62" s="21"/>
     </row>
@@ -22988,7 +22988,7 @@
       </c>
       <c r="G63" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F63)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H63" s="21"/>
     </row>
@@ -23010,7 +23010,7 @@
       </c>
       <c r="G64" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F64)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H64" s="21"/>
     </row>
@@ -23032,7 +23032,7 @@
       </c>
       <c r="G65" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F65)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H65" s="21"/>
     </row>
@@ -23054,7 +23054,7 @@
       </c>
       <c r="G66" s="22" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(F66)</f>
-        <v>qlLiborSwap - Unhandled currency AUD</v>
+        <v/>
       </c>
       <c r="H66" s="21"/>
     </row>
@@ -23305,7 +23305,7 @@
       </c>
       <c r="Q5" s="370" t="str">
         <f>_xll.RData(Q6:Q14,R5:S5,"RTFEED:IDN",,,R6)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="R5" s="370" t="s">
         <v>227</v>
@@ -23535,7 +23535,7 @@
       </c>
       <c r="V8" s="458">
         <f>_xll.qlQuoteValue(L8)</f>
-        <v>2.6699999999999998E-2</v>
+        <v>2.69E-2</v>
       </c>
       <c r="W8" s="365"/>
     </row>
@@ -23609,7 +23609,7 @@
       </c>
       <c r="V9" s="458">
         <f>_xll.qlQuoteValue(L9)</f>
-        <v>2.69E-2</v>
+        <v>2.7000000000000003E-2</v>
       </c>
       <c r="W9" s="365"/>
     </row>
@@ -23751,7 +23751,7 @@
       </c>
       <c r="V11" s="458">
         <f>_xll.qlQuoteValue(L11)</f>
-        <v>2.7000000000000003E-2</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="W11" s="365"/>
     </row>
@@ -23823,9 +23823,9 @@
         <f>IF(S12,_xll.qlIndexAddFixings(P12,R12,S12/100,TRUE),NA())</f>
         <v>1</v>
       </c>
-      <c r="V12" s="458" t="e">
+      <c r="V12" s="458">
         <f>_xll.qlQuoteValue(L12)</f>
-        <v>#NUM!</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="W12" s="365"/>
     </row>
@@ -24083,8 +24083,8 @@
         <v>AudBBSWSwapForBasisCalc1Y</v>
       </c>
       <c r="F4" s="406" t="str">
-        <f>_xll.qlSwapIndex($E4,FixingType,C4,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!K9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWswapForBasisCalc1Y#0004</v>
+        <f>_xll.qlSwapIndex($E4,FixingType,C4,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>AudBBSWSwapForBasisCalc1Y#0012</v>
       </c>
       <c r="G4" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -24105,8 +24105,8 @@
         <v>AudBBSWSwapForBasisCalc2Y</v>
       </c>
       <c r="F5" s="406" t="str">
-        <f>_xll.qlSwapIndex($E5,FixingType,C5,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!K10,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWswapForBasisCalc2Y#0008</v>
+        <f>_xll.qlSwapIndex($E5,FixingType,C5,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>AudBBSWSwapForBasisCalc2Y#0003</v>
       </c>
       <c r="G5" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -24127,8 +24127,8 @@
         <v>AudBBSWSwapForBasisCalc3Y</v>
       </c>
       <c r="F6" s="406" t="str">
-        <f>_xll.qlSwapIndex($E6,FixingType,C6,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!K11,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWswapForBasisCalc3Y#0008</v>
+        <f>_xll.qlSwapIndex($E6,FixingType,C6,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>AudBBSWSwapForBasisCalc3Y#0003</v>
       </c>
       <c r="G6" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -24149,8 +24149,8 @@
         <v>AudBBSWSwapForBasisCalc4Y</v>
       </c>
       <c r="F7" s="406" t="str">
-        <f>_xll.qlSwapIndex($E7,FixingType,C7,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!K12,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWswapForBasisCalc4Y#0008</v>
+        <f>_xll.qlSwapIndex($E7,FixingType,C7,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>AudBBSWSwapForBasisCalc4Y#0003</v>
       </c>
       <c r="G7" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -24878,7 +24878,7 @@
       <c r="N4" s="82"/>
       <c r="O4" s="220" t="str">
         <f>_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:12:37</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="P4" s="217" t="s">
         <v>162</v>
@@ -25174,7 +25174,7 @@
       </c>
       <c r="Y8" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F8,X8/100,Trigger)</f>
-        <v>9.9999999999995925E-6</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="126"/>
       <c r="AB8"/>
@@ -25376,7 +25376,7 @@
       </c>
       <c r="Y11" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="126"/>
     </row>
@@ -25443,7 +25443,7 @@
       </c>
       <c r="Y12" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
-        <v>-2.4999999999997247E-5</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="126"/>
     </row>
@@ -25711,7 +25711,7 @@
       </c>
       <c r="Y16" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F16,X16/100,Trigger)</f>
-        <v>-1.4999999999997654E-5</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="126"/>
     </row>
@@ -25912,7 +25912,7 @@
       </c>
       <c r="Y19" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F19,X19/100,Trigger)</f>
-        <v>3.4999999999996839E-5</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="126"/>
     </row>
@@ -26314,7 +26314,7 @@
       </c>
       <c r="Y25" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F25,X25/100,Trigger)</f>
-        <v>4.9999999999997963E-5</v>
+        <v>0</v>
       </c>
       <c r="Z25" s="126"/>
     </row>
@@ -26716,7 +26716,7 @@
       </c>
       <c r="Y31" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F31,X31/100,Trigger)</f>
-        <v>5.0000000000001432E-5</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="126"/>
     </row>
@@ -26984,7 +26984,7 @@
       </c>
       <c r="Y35" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F35,X35/100,Trigger)</f>
-        <v>1.5000000000000083E-4</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="126"/>
     </row>
@@ -28832,7 +28832,7 @@
       <c r="N4" s="82"/>
       <c r="O4" s="220" t="str">
         <f>_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:12:38</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="P4" s="217" t="s">
         <v>162</v>
@@ -30351,7 +30351,7 @@
       </c>
       <c r="Y25" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F25,X25/100,Trigger)</f>
-        <v>4.9999999999997963E-5</v>
+        <v>0</v>
       </c>
       <c r="Z25" s="126"/>
     </row>
@@ -30777,7 +30777,7 @@
       </c>
       <c r="Y31" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F31,X31/100,Trigger)</f>
-        <v>5.0000000000004902E-5</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="126"/>
     </row>
@@ -31061,7 +31061,7 @@
       </c>
       <c r="Y35" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F35,X35/100,Trigger)</f>
-        <v>9.9999999999999395E-5</v>
+        <v>0</v>
       </c>
       <c r="Z35" s="126"/>
     </row>
@@ -31345,7 +31345,7 @@
       </c>
       <c r="Y39" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F39,X39/100,Trigger)</f>
-        <v>2.9999999999999818E-4</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="126"/>
     </row>
@@ -31629,7 +31629,7 @@
       </c>
       <c r="Y43" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F43,X43/100,Trigger)</f>
-        <v>3.2999999999999696E-4</v>
+        <v>0</v>
       </c>
       <c r="Z43" s="126"/>
     </row>
@@ -31700,7 +31700,7 @@
       </c>
       <c r="Y44" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F44,X44/100,Trigger)</f>
-        <v>3.8000000000000533E-4</v>
+        <v>0</v>
       </c>
       <c r="Z44" s="126"/>
     </row>
@@ -31771,7 +31771,7 @@
       </c>
       <c r="Y45" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F45,X45/100,Trigger)</f>
-        <v>4.3000000000000677E-4</v>
+        <v>0</v>
       </c>
       <c r="Z45" s="126"/>
     </row>
@@ -31842,7 +31842,7 @@
       </c>
       <c r="Y46" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>4.4999999999999901E-4</v>
+        <v>0</v>
       </c>
       <c r="Z46" s="126"/>
     </row>
@@ -31913,7 +31913,7 @@
       </c>
       <c r="Y47" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>4.9999999999999351E-4</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="126"/>
     </row>
@@ -31984,7 +31984,7 @@
       </c>
       <c r="Y48" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>5.3000000000000269E-4</v>
+        <v>0</v>
       </c>
       <c r="Z48" s="126"/>
     </row>
@@ -32055,7 +32055,7 @@
       </c>
       <c r="Y49" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>5.5000000000000188E-4</v>
+        <v>0</v>
       </c>
       <c r="Z49" s="126"/>
     </row>
@@ -32126,7 +32126,7 @@
       </c>
       <c r="Y50" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>5.7999999999999718E-4</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="126"/>
     </row>
@@ -32197,7 +32197,7 @@
       </c>
       <c r="Y51" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>5.0000000000000738E-4</v>
+        <v>0</v>
       </c>
       <c r="Z51" s="126"/>
     </row>
@@ -32268,7 +32268,7 @@
       </c>
       <c r="Y52" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>5.0000000000000738E-4</v>
+        <v>0</v>
       </c>
       <c r="Z52" s="126"/>
     </row>
@@ -32410,7 +32410,7 @@
       </c>
       <c r="Y54" s="136">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>5.3000000000000963E-4</v>
+        <v>0</v>
       </c>
       <c r="Z54" s="126"/>
     </row>
@@ -32962,7 +32962,7 @@
       <c r="Q3" s="169"/>
       <c r="R3" s="168">
         <f>_xll.ohTrigger(R5:R18)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" s="126"/>
       <c r="T3" s="12"/>
@@ -32992,7 +32992,7 @@
       <c r="I4" s="165"/>
       <c r="J4" s="134" t="str">
         <f>_xll.RData(J6:J22,K4:L4,,ReutersRtMode,,K6)</f>
-        <v>Updated at 09:21:40</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="K4" s="134" t="s">
         <v>162</v>
@@ -34371,7 +34371,7 @@
       <c r="M4" s="59"/>
       <c r="N4" s="473" t="str">
         <f>_xll.RData(N5:N19,O4:R4,"RTFEED:IDN",ReutersRtMode,,O5)</f>
-        <v>Updated at 09:13:49</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="O4" s="166" t="s">
         <v>162</v>
@@ -34471,7 +34471,7 @@
       </c>
       <c r="X5" s="155">
         <f>_xll.qlSimpleQuoteSetValue(E5,W5/100,Trigger)</f>
-        <v>4.9999999999997963E-5</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="126"/>
       <c r="Z5" s="12"/>
@@ -34543,7 +34543,7 @@
       </c>
       <c r="X6" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E6,W6/100,Trigger)</f>
-        <v>-4.9999999999997963E-5</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="126"/>
       <c r="Z6" s="12"/>
@@ -34831,7 +34831,7 @@
       </c>
       <c r="X10" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E10,W10/100,Trigger)</f>
-        <v>4.9999999999997963E-5</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="126"/>
       <c r="Z10" s="12"/>
@@ -34904,7 +34904,7 @@
       </c>
       <c r="X11" s="477">
         <f>_xll.qlSimpleQuoteSetValue(E11,W11/100,Trigger)</f>
-        <v>-9.9999999999999395E-5</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="126"/>
       <c r="Z11" s="12"/>
@@ -35050,7 +35050,7 @@
       </c>
       <c r="X13" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E13,W13/100,Trigger)</f>
-        <v>-9.9999999999999395E-5</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="126"/>
       <c r="Z13" s="12"/>
@@ -35123,7 +35123,7 @@
       </c>
       <c r="X14" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E14,W14/100,Trigger)</f>
-        <v>-2.0000000000000226E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="126"/>
       <c r="Z14" s="12"/>
@@ -35196,7 +35196,7 @@
       </c>
       <c r="X15" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E15,W15/100,Trigger)</f>
-        <v>-1.9999999999999879E-4</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="126"/>
       <c r="Z15" s="12"/>
@@ -35269,7 +35269,7 @@
       </c>
       <c r="X16" s="136">
         <f>_xll.qlSimpleQuoteSetValue(E16,W16/100,Trigger)</f>
-        <v>-1.9999999999999879E-4</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="126"/>
       <c r="Z16" s="12"/>
@@ -35794,7 +35794,7 @@
       </c>
       <c r="O5" s="134" t="str">
         <f>_xll.RData(O6:O17,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
-        <v>Updated at 09:12:36</v>
+        <v>Updated at 14:39:37</v>
       </c>
       <c r="P5" s="188" t="s">
         <v>195</v>
@@ -36045,7 +36045,7 @@
       </c>
       <c r="AO7" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN7)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MM4_Quote'</v>
+        <v/>
       </c>
       <c r="AP7" s="213"/>
     </row>
@@ -36150,7 +36150,7 @@
       </c>
       <c r="AO8" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN8)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MN4_Quote'</v>
+        <v/>
       </c>
       <c r="AP8" s="213"/>
     </row>
@@ -36255,7 +36255,7 @@
       </c>
       <c r="AO9" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN9)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MQ4_Quote'</v>
+        <v/>
       </c>
       <c r="AP9" s="213"/>
       <c r="AQ9" s="341"/>
@@ -36361,7 +36361,7 @@
       </c>
       <c r="AO10" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN10)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MU4_Quote'</v>
+        <v/>
       </c>
       <c r="AP10" s="213"/>
     </row>
@@ -36466,7 +36466,7 @@
       </c>
       <c r="AO11" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN11)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MV4_Quote'</v>
+        <v/>
       </c>
       <c r="AP11" s="213"/>
     </row>
@@ -36571,7 +36571,7 @@
       </c>
       <c r="AO12" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN12)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MX4_Quote'</v>
+        <v/>
       </c>
       <c r="AP12" s="213"/>
     </row>
@@ -36676,7 +36676,7 @@
       </c>
       <c r="AO13" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN13)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MZ4_Quote'</v>
+        <v/>
       </c>
       <c r="AP13" s="213"/>
     </row>
@@ -36781,7 +36781,7 @@
       </c>
       <c r="AO14" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN14)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MF5_Quote'</v>
+        <v/>
       </c>
       <c r="AP14" s="213"/>
     </row>
@@ -36886,7 +36886,7 @@
       </c>
       <c r="AO15" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN15)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MG5_Quote'</v>
+        <v/>
       </c>
       <c r="AP15" s="213"/>
     </row>
@@ -36991,7 +36991,7 @@
       </c>
       <c r="AO16" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN16)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MH5_Quote'</v>
+        <v/>
       </c>
       <c r="AP16" s="213"/>
     </row>
@@ -37096,7 +37096,7 @@
       </c>
       <c r="AO17" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN17)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MJ5_Quote'</v>
+        <v/>
       </c>
       <c r="AP17" s="213"/>
     </row>
@@ -37156,7 +37156,7 @@
       </c>
       <c r="AO18" s="46" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(AN18)</f>
-        <v>qlFuturesConvAdjustmentQuote - Error converting parameter 'FuturesQuote' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'AUDFUT1MK5_Quote'</v>
+        <v/>
       </c>
       <c r="AP18" s="213"/>
     </row>
@@ -37381,7 +37381,7 @@
       <c r="Y4" s="83"/>
       <c r="Z4" s="168">
         <f>_xll.ohTrigger(Z6:Z47)</f>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="213"/>
       <c r="AB4" s="12"/>
@@ -37440,7 +37440,7 @@
       </c>
       <c r="O5" s="220" t="str">
         <f>_xll.RData(O6:O47,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
-        <v>Updated at 09:22:05</v>
+        <v>Updated at 14:43:55</v>
       </c>
       <c r="P5" s="217" t="s">
         <v>195</v>
@@ -37592,7 +37592,7 @@
       </c>
       <c r="AH6" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG6,IborIndex,AF6,F6,Volatility,MeanReversion,Permanent,AND(ISERROR(Z6),ISERROR(FuturesHWConvAdj!Q5:Q6)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI6" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH6)</f>
@@ -37689,7 +37689,7 @@
       </c>
       <c r="AH7" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG7,IborIndex,AF7,F7,Volatility,MeanReversion,Permanent,AND(ISERROR(Z7),ISERROR(FuturesHWConvAdj!Q6:Q7)),ObjectOverwrite)</f>
-        <v>AUDFUT3MN4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MN4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI7" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH7)</f>
@@ -37786,7 +37786,7 @@
       </c>
       <c r="AH8" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG8,IborIndex,AF8,F8,Volatility,MeanReversion,Permanent,AND(ISERROR(Z8),ISERROR(FuturesHWConvAdj!Q7:Q8)),ObjectOverwrite)</f>
-        <v>AUDFUT3MQ4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MQ4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI8" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH8)</f>
@@ -37844,7 +37844,7 @@
         <v>97.34</v>
       </c>
       <c r="S9" s="137">
-        <v>0</v>
+        <v>97.33</v>
       </c>
       <c r="T9" s="137">
         <v>97.34</v>
@@ -37883,7 +37883,7 @@
       </c>
       <c r="AH9" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG9,IborIndex,AF9,F9,Volatility,MeanReversion,Permanent,AND(ISERROR(Z9),ISERROR(FuturesHWConvAdj!Q8:Q9)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI9" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH9)</f>
@@ -37981,7 +37981,7 @@
       </c>
       <c r="AH10" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG10,IborIndex,AF10,F10,Volatility,MeanReversion,Permanent,AND(ISERROR(Z10),ISERROR(FuturesHWConvAdj!Q9:Q10)),ObjectOverwrite)</f>
-        <v>AUDFUT3MV4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MV4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI10" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH10)</f>
@@ -38078,7 +38078,7 @@
       </c>
       <c r="AH11" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG11,IborIndex,AF11,F11,Volatility,MeanReversion,Permanent,AND(ISERROR(Z11),ISERROR(FuturesHWConvAdj!Q10:Q11)),ObjectOverwrite)</f>
-        <v>AUDFUT3MX4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MX4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI11" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH11)</f>
@@ -38130,20 +38130,20 @@
         <v>41984</v>
       </c>
       <c r="Q12" s="137">
-        <v>97.33</v>
+        <v>97.34</v>
       </c>
       <c r="R12" s="137">
-        <v>97.34</v>
+        <v>97.35</v>
       </c>
       <c r="S12" s="137">
-        <v>0</v>
+        <v>97.35</v>
       </c>
       <c r="T12" s="137">
         <v>97.33</v>
       </c>
       <c r="U12" s="141">
         <f>_xll.qlMidSafe($Q12,$R12)</f>
-        <v>97.335000000000008</v>
+        <v>97.344999999999999</v>
       </c>
       <c r="V12" s="139"/>
       <c r="W12" s="200">
@@ -38151,11 +38151,11 @@
       </c>
       <c r="X12" s="139"/>
       <c r="Y12" s="199">
-        <v>97.335000000000008</v>
+        <v>97.344999999999999</v>
       </c>
       <c r="Z12" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F12,Y12,Trigger)</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA12" s="21"/>
       <c r="AB12" s="12"/>
@@ -38175,7 +38175,7 @@
       </c>
       <c r="AH12" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG12,IborIndex,AF12,F12,Volatility,MeanReversion,Permanent,AND(ISERROR(Z12),ISERROR(FuturesHWConvAdj!Q11:Q12)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ4ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ4ConvAdj_Quote#0001</v>
       </c>
       <c r="AI12" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH12)</f>
@@ -38272,7 +38272,7 @@
       </c>
       <c r="AH13" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG13,IborIndex,AF13,F13,Volatility,MeanReversion,Permanent,AND(ISERROR(Z13),ISERROR(FuturesHWConvAdj!Q12:Q13)),ObjectOverwrite)</f>
-        <v>AUDFUT3MF5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MF5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI13" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH13)</f>
@@ -38369,7 +38369,7 @@
       </c>
       <c r="AH14" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG14,IborIndex,AF14,F14,Volatility,MeanReversion,Permanent,AND(ISERROR(Z14),ISERROR(FuturesHWConvAdj!Q13:Q14)),ObjectOverwrite)</f>
-        <v>AUDFUT3MG5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MG5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI14" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH14)</f>
@@ -38421,20 +38421,20 @@
         <v>42075</v>
       </c>
       <c r="Q15" s="137">
-        <v>97.29</v>
+        <v>97.3</v>
       </c>
       <c r="R15" s="137">
-        <v>97.3</v>
+        <v>97.31</v>
       </c>
       <c r="S15" s="137">
-        <v>97.29</v>
+        <v>97.31</v>
       </c>
       <c r="T15" s="137">
         <v>97.3</v>
       </c>
       <c r="U15" s="141">
         <f>_xll.qlMidSafe($Q15,$R15)</f>
-        <v>97.295000000000002</v>
+        <v>97.305000000000007</v>
       </c>
       <c r="V15" s="139"/>
       <c r="W15" s="200">
@@ -38442,11 +38442,11 @@
       </c>
       <c r="X15" s="139"/>
       <c r="Y15" s="199">
-        <v>97.295000000000002</v>
+        <v>97.305000000000007</v>
       </c>
       <c r="Z15" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F15,Y15,Trigger)</f>
-        <v>0</v>
+        <v>1.0000000000005116E-2</v>
       </c>
       <c r="AA15" s="21"/>
       <c r="AB15" s="12"/>
@@ -38466,7 +38466,7 @@
       </c>
       <c r="AH15" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG15,IborIndex,AF15,F15,Volatility,MeanReversion,Permanent,AND(ISERROR(Z15),ISERROR(FuturesHWConvAdj!Q14:Q15)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI15" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH15)</f>
@@ -38563,7 +38563,7 @@
       </c>
       <c r="AH16" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG16,IborIndex,AF16,F16,Volatility,MeanReversion,Permanent,AND(ISERROR(Z16),ISERROR(FuturesHWConvAdj!Q15:Q16)),ObjectOverwrite)</f>
-        <v>AUDFUT3MJ5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MJ5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI16" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH16)</f>
@@ -38660,7 +38660,7 @@
       </c>
       <c r="AH17" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG17,IborIndex,AF17,F17,Volatility,MeanReversion,Permanent,AND(ISERROR(Z17),ISERROR(FuturesHWConvAdj!Q16:Q17)),ObjectOverwrite)</f>
-        <v>AUDFUT3MK5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MK5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI17" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH17)</f>
@@ -38757,7 +38757,7 @@
       </c>
       <c r="AH18" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG18,IborIndex,AF18,F18,Volatility,MeanReversion,Permanent,AND(ISERROR(Z18),ISERROR(FuturesHWConvAdj!Q17:Q18)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI18" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH18)</f>
@@ -38809,20 +38809,20 @@
         <v>42257</v>
       </c>
       <c r="Q19" s="137">
-        <v>97.1</v>
+        <v>97.11</v>
       </c>
       <c r="R19" s="137">
+        <v>97.12</v>
+      </c>
+      <c r="S19" s="137">
         <v>97.11</v>
-      </c>
-      <c r="S19" s="137">
-        <v>0</v>
       </c>
       <c r="T19" s="137">
         <v>97.11</v>
       </c>
       <c r="U19" s="141">
         <f>_xll.qlMidSafe($Q19,$R19)</f>
-        <v>97.10499999999999</v>
+        <v>97.115000000000009</v>
       </c>
       <c r="V19" s="139"/>
       <c r="W19" s="200">
@@ -38830,11 +38830,11 @@
       </c>
       <c r="X19" s="139"/>
       <c r="Y19" s="199">
-        <v>97.10499999999999</v>
+        <v>97.115000000000009</v>
       </c>
       <c r="Z19" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F19,Y19,Trigger)</f>
-        <v>0</v>
+        <v>1.0000000000019327E-2</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="12"/>
@@ -38854,7 +38854,7 @@
       </c>
       <c r="AH19" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG19,IborIndex,AF19,F19,Volatility,MeanReversion,Permanent,AND(ISERROR(Z19),ISERROR(FuturesHWConvAdj!Q18:Q19)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI19" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH19)</f>
@@ -38906,20 +38906,20 @@
         <v>42348</v>
       </c>
       <c r="Q20" s="137">
-        <v>96.99</v>
+        <v>97</v>
       </c>
       <c r="R20" s="137">
-        <v>97</v>
+        <v>97.01</v>
       </c>
       <c r="S20" s="137">
-        <v>0</v>
+        <v>97.01</v>
       </c>
       <c r="T20" s="137">
         <v>97</v>
       </c>
       <c r="U20" s="141">
         <f>_xll.qlMidSafe($Q20,$R20)</f>
-        <v>96.995000000000005</v>
+        <v>97.004999999999995</v>
       </c>
       <c r="V20" s="139"/>
       <c r="W20" s="200">
@@ -38927,11 +38927,11 @@
       </c>
       <c r="X20" s="139"/>
       <c r="Y20" s="199">
-        <v>96.995000000000005</v>
+        <v>97.004999999999995</v>
       </c>
       <c r="Z20" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20,Trigger)</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA20" s="21"/>
       <c r="AB20" s="12"/>
@@ -38951,7 +38951,7 @@
       </c>
       <c r="AH20" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG20,IborIndex,AF20,F20,Volatility,MeanReversion,Permanent,AND(ISERROR(Z20),ISERROR(FuturesHWConvAdj!Q19:Q20)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ5ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ5ConvAdj_Quote#0001</v>
       </c>
       <c r="AI20" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH20)</f>
@@ -39003,20 +39003,20 @@
         <v>42439</v>
       </c>
       <c r="Q21" s="137">
-        <v>96.89</v>
+        <v>96.9</v>
       </c>
       <c r="R21" s="137">
-        <v>96.9</v>
+        <v>96.92</v>
       </c>
       <c r="S21" s="137">
-        <v>0</v>
+        <v>96.91</v>
       </c>
       <c r="T21" s="137">
         <v>96.9</v>
       </c>
       <c r="U21" s="141">
         <f>_xll.qlMidSafe($Q21,$R21)</f>
-        <v>96.89500000000001</v>
+        <v>96.91</v>
       </c>
       <c r="V21" s="139"/>
       <c r="W21" s="200">
@@ -39024,11 +39024,11 @@
       </c>
       <c r="X21" s="139"/>
       <c r="Y21" s="199">
-        <v>96.89500000000001</v>
+        <v>96.91</v>
       </c>
       <c r="Z21" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F21,Y21,Trigger)</f>
-        <v>0</v>
+        <v>1.4999999999986358E-2</v>
       </c>
       <c r="AA21" s="21"/>
       <c r="AB21" s="12"/>
@@ -39048,7 +39048,7 @@
       </c>
       <c r="AH21" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG21,IborIndex,AF21,F21,Volatility,MeanReversion,Permanent,AND(ISERROR(Z21),ISERROR(FuturesHWConvAdj!Q20:Q21)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH6ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH6ConvAdj_Quote#0001</v>
       </c>
       <c r="AI21" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH21)</f>
@@ -39100,20 +39100,20 @@
         <v>42530</v>
       </c>
       <c r="Q22" s="137">
-        <v>96.79</v>
+        <v>96.81</v>
       </c>
       <c r="R22" s="137">
+        <v>96.83</v>
+      </c>
+      <c r="S22" s="137">
         <v>96.81</v>
-      </c>
-      <c r="S22" s="137">
-        <v>0</v>
       </c>
       <c r="T22" s="137">
         <v>96.8</v>
       </c>
       <c r="U22" s="141">
         <f>_xll.qlMidSafe($Q22,$R22)</f>
-        <v>96.800000000000011</v>
+        <v>96.82</v>
       </c>
       <c r="V22" s="139"/>
       <c r="W22" s="200">
@@ -39121,11 +39121,11 @@
       </c>
       <c r="X22" s="139"/>
       <c r="Y22" s="199">
-        <v>96.800000000000011</v>
+        <v>96.82</v>
       </c>
       <c r="Z22" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F22,Y22,Trigger)</f>
-        <v>0</v>
+        <v>1.999999999998181E-2</v>
       </c>
       <c r="AA22" s="21"/>
       <c r="AB22" s="12"/>
@@ -39145,7 +39145,7 @@
       </c>
       <c r="AH22" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG22,IborIndex,AF22,F22,Volatility,MeanReversion,Permanent,AND(ISERROR(Z22),ISERROR(FuturesHWConvAdj!Q21:Q22)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM6ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM6ConvAdj_Quote#0001</v>
       </c>
       <c r="AI22" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH22)</f>
@@ -39197,7 +39197,7 @@
         <v>42621</v>
       </c>
       <c r="Q23" s="137">
-        <v>96.69</v>
+        <v>96.71</v>
       </c>
       <c r="R23" s="137">
         <v>96.73</v>
@@ -39210,7 +39210,7 @@
       </c>
       <c r="U23" s="141">
         <f>_xll.qlMidSafe($Q23,$R23)</f>
-        <v>96.710000000000008</v>
+        <v>96.72</v>
       </c>
       <c r="V23" s="139"/>
       <c r="W23" s="200">
@@ -39218,11 +39218,11 @@
       </c>
       <c r="X23" s="139"/>
       <c r="Y23" s="199">
-        <v>96.710000000000008</v>
+        <v>96.72</v>
       </c>
       <c r="Z23" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F23,Y23,Trigger)</f>
-        <v>0</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="AA23" s="21"/>
       <c r="AB23" s="12"/>
@@ -39242,7 +39242,7 @@
       </c>
       <c r="AH23" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG23,IborIndex,AF23,F23,Volatility,MeanReversion,Permanent,AND(ISERROR(Z23),ISERROR(FuturesHWConvAdj!Q22:Q23)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU6ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU6ConvAdj_Quote#0001</v>
       </c>
       <c r="AI23" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH23)</f>
@@ -39294,10 +39294,10 @@
         <v>42712</v>
       </c>
       <c r="Q24" s="137">
-        <v>96.58</v>
+        <v>96.61</v>
       </c>
       <c r="R24" s="137">
-        <v>96.63</v>
+        <v>96.64</v>
       </c>
       <c r="S24" s="137">
         <v>0</v>
@@ -39307,7 +39307,7 @@
       </c>
       <c r="U24" s="141">
         <f>_xll.qlMidSafe($Q24,$R24)</f>
-        <v>96.60499999999999</v>
+        <v>96.625</v>
       </c>
       <c r="V24" s="139"/>
       <c r="W24" s="200">
@@ -39315,11 +39315,11 @@
       </c>
       <c r="X24" s="139"/>
       <c r="Y24" s="199">
-        <v>96.60499999999999</v>
+        <v>96.625</v>
       </c>
       <c r="Z24" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F24,Y24,Trigger)</f>
-        <v>-5.0000000000096634E-3</v>
+        <v>2.0000000000010232E-2</v>
       </c>
       <c r="AA24" s="21"/>
       <c r="AB24" s="12"/>
@@ -39339,7 +39339,7 @@
       </c>
       <c r="AH24" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG24,IborIndex,AF24,F24,Volatility,MeanReversion,Permanent,AND(ISERROR(Z24),ISERROR(FuturesHWConvAdj!Q23:Q24)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ6ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ6ConvAdj_Quote#0001</v>
       </c>
       <c r="AI24" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH24)</f>
@@ -39391,7 +39391,7 @@
         <v>42803</v>
       </c>
       <c r="Q25" s="137">
-        <v>96.46</v>
+        <v>96.51</v>
       </c>
       <c r="R25" s="137">
         <v>96.55</v>
@@ -39404,7 +39404,7 @@
       </c>
       <c r="U25" s="141">
         <f>_xll.qlMidSafe($Q25,$R25)</f>
-        <v>96.504999999999995</v>
+        <v>96.53</v>
       </c>
       <c r="V25" s="139"/>
       <c r="W25" s="200">
@@ -39412,11 +39412,11 @@
       </c>
       <c r="X25" s="139"/>
       <c r="Y25" s="199">
-        <v>96.504999999999995</v>
+        <v>96.53</v>
       </c>
       <c r="Z25" s="141">
         <f>_xll.qlSimpleQuoteSetValue(F25,Y25,Trigger)</f>
-        <v>-4.9999999999954525E-3</v>
+        <v>2.5000000000005684E-2</v>
       </c>
       <c r="AA25" s="21"/>
       <c r="AB25" s="12"/>
@@ -39436,7 +39436,7 @@
       </c>
       <c r="AH25" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG25,IborIndex,AF25,F25,Volatility,MeanReversion,Permanent,AND(ISERROR(Z25),ISERROR(FuturesHWConvAdj!Q24:Q25)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH7ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH7ConvAdj_Quote#0001</v>
       </c>
       <c r="AI25" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH25)</f>
@@ -39491,7 +39491,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="137">
-        <v>0</v>
+        <v>96.49</v>
       </c>
       <c r="S26" s="137">
         <v>0</v>
@@ -39533,7 +39533,7 @@
       </c>
       <c r="AH26" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG26,IborIndex,AF26,F26,Volatility,MeanReversion,Permanent,AND(ISERROR(Z26),ISERROR(FuturesHWConvAdj!Q25:Q26)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM7ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM7ConvAdj_Quote#0001</v>
       </c>
       <c r="AI26" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH26)</f>
@@ -39630,7 +39630,7 @@
       </c>
       <c r="AH27" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG27,IborIndex,AF27,F27,Volatility,MeanReversion,Permanent,AND(ISERROR(Z27),ISERROR(FuturesHWConvAdj!Q26:Q27)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU7ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU7ConvAdj_Quote#0001</v>
       </c>
       <c r="AI27" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH27)</f>
@@ -39727,7 +39727,7 @@
       </c>
       <c r="AH28" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG28,IborIndex,AF28,F28,Volatility,MeanReversion,Permanent,AND(ISERROR(Z28),ISERROR(FuturesHWConvAdj!Q27:Q28)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ7ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ7ConvAdj_Quote#0001</v>
       </c>
       <c r="AI28" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH28)</f>
@@ -39824,7 +39824,7 @@
       </c>
       <c r="AH29" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG29,IborIndex,AF29,F29,Volatility,MeanReversion,Permanent,AND(ISERROR(Z29),ISERROR(FuturesHWConvAdj!Q28:Q29)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH8ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH8ConvAdj_Quote#0001</v>
       </c>
       <c r="AI29" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH29)</f>
@@ -39921,7 +39921,7 @@
       </c>
       <c r="AH30" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG30,IborIndex,AF30,F30,Volatility,MeanReversion,Permanent,AND(ISERROR(Z30),ISERROR(FuturesHWConvAdj!Q29:Q30)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM8ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM8ConvAdj_Quote#0001</v>
       </c>
       <c r="AI30" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH30)</f>
@@ -40018,7 +40018,7 @@
       </c>
       <c r="AH31" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG31,IborIndex,AF31,F31,Volatility,MeanReversion,Permanent,AND(ISERROR(Z31),ISERROR(FuturesHWConvAdj!Q30:Q31)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU8ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU8ConvAdj_Quote#0001</v>
       </c>
       <c r="AI31" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH31)</f>
@@ -40115,7 +40115,7 @@
       </c>
       <c r="AH32" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG32,IborIndex,AF32,F32,Volatility,MeanReversion,Permanent,AND(ISERROR(Z32),ISERROR(FuturesHWConvAdj!Q31:Q32)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ8ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ8ConvAdj_Quote#0001</v>
       </c>
       <c r="AI32" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH32)</f>
@@ -40212,7 +40212,7 @@
       </c>
       <c r="AH33" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG33,IborIndex,AF33,F33,Volatility,MeanReversion,Permanent,AND(ISERROR(Z33),ISERROR(FuturesHWConvAdj!Q32:Q33)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH9ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH9ConvAdj_Quote#0001</v>
       </c>
       <c r="AI33" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH33)</f>
@@ -40309,7 +40309,7 @@
       </c>
       <c r="AH34" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG34,IborIndex,AF34,F34,Volatility,MeanReversion,Permanent,AND(ISERROR(Z34),ISERROR(FuturesHWConvAdj!Q33:Q34)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM9ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM9ConvAdj_Quote#0001</v>
       </c>
       <c r="AI34" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH34)</f>
@@ -40406,7 +40406,7 @@
       </c>
       <c r="AH35" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG35,IborIndex,AF35,F35,Volatility,MeanReversion,Permanent,AND(ISERROR(Z35),ISERROR(FuturesHWConvAdj!Q34:Q35)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU9ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU9ConvAdj_Quote#0001</v>
       </c>
       <c r="AI35" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH35)</f>
@@ -40503,7 +40503,7 @@
       </c>
       <c r="AH36" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG36,IborIndex,AF36,F36,Volatility,MeanReversion,Permanent,AND(ISERROR(Z36),ISERROR(FuturesHWConvAdj!Q35:Q36)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ9ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ9ConvAdj_Quote#0001</v>
       </c>
       <c r="AI36" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH36)</f>
@@ -40600,7 +40600,7 @@
       </c>
       <c r="AH37" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG37,IborIndex,AF37,F37,Volatility,MeanReversion,Permanent,AND(ISERROR(Z37),ISERROR(FuturesHWConvAdj!Q36:Q37)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH0ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH0ConvAdj_Quote#0001</v>
       </c>
       <c r="AI37" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH37)</f>
@@ -40697,7 +40697,7 @@
       </c>
       <c r="AH38" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG38,IborIndex,AF38,F38,Volatility,MeanReversion,Permanent,AND(ISERROR(Z38),ISERROR(FuturesHWConvAdj!Q37:Q38)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM0ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM0ConvAdj_Quote#0001</v>
       </c>
       <c r="AI38" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH38)</f>
@@ -40794,7 +40794,7 @@
       </c>
       <c r="AH39" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG39,IborIndex,AF39,F39,Volatility,MeanReversion,Permanent,AND(ISERROR(Z39),ISERROR(FuturesHWConvAdj!Q38:Q39)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU0ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU0ConvAdj_Quote#0001</v>
       </c>
       <c r="AI39" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH39)</f>
@@ -40891,7 +40891,7 @@
       </c>
       <c r="AH40" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG40,IborIndex,AF40,F40,Volatility,MeanReversion,Permanent,AND(ISERROR(Z40),ISERROR(FuturesHWConvAdj!Q39:Q40)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ0ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ0ConvAdj_Quote#0001</v>
       </c>
       <c r="AI40" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH40)</f>
@@ -40988,7 +40988,7 @@
       </c>
       <c r="AH41" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG41,IborIndex,AF41,F41,Volatility,MeanReversion,Permanent,AND(ISERROR(Z41),ISERROR(FuturesHWConvAdj!Q40:Q41)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH1ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH1ConvAdj_Quote#0001</v>
       </c>
       <c r="AI41" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH41)</f>
@@ -41085,7 +41085,7 @@
       </c>
       <c r="AH42" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG42,IborIndex,AF42,F42,Volatility,MeanReversion,Permanent,AND(ISERROR(Z42),ISERROR(FuturesHWConvAdj!Q41:Q42)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM1ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM1ConvAdj_Quote#0001</v>
       </c>
       <c r="AI42" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH42)</f>
@@ -41182,7 +41182,7 @@
       </c>
       <c r="AH43" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG43,IborIndex,AF43,F43,Volatility,MeanReversion,Permanent,AND(ISERROR(Z43),ISERROR(FuturesHWConvAdj!Q42:Q43)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU1ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU1ConvAdj_Quote#0001</v>
       </c>
       <c r="AI43" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH43)</f>
@@ -41279,7 +41279,7 @@
       </c>
       <c r="AH44" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG44,IborIndex,AF44,F44,Volatility,MeanReversion,Permanent,AND(ISERROR(Z44),ISERROR(FuturesHWConvAdj!Q43:Q44)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ1ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MZ1ConvAdj_Quote#0001</v>
       </c>
       <c r="AI44" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH44)</f>
@@ -41376,7 +41376,7 @@
       </c>
       <c r="AH45" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG45,IborIndex,AF45,F45,Volatility,MeanReversion,Permanent,AND(ISERROR(Z45),ISERROR(FuturesHWConvAdj!Q44:Q45)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH2ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MH2ConvAdj_Quote#0001</v>
       </c>
       <c r="AI45" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH45)</f>
@@ -41473,7 +41473,7 @@
       </c>
       <c r="AH46" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG46,IborIndex,AF46,F46,Volatility,MeanReversion,Permanent,AND(ISERROR(Z46),ISERROR(FuturesHWConvAdj!Q45:Q46)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM2ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MM2ConvAdj_Quote#0001</v>
       </c>
       <c r="AI46" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH46)</f>
@@ -41570,7 +41570,7 @@
       </c>
       <c r="AH47" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG47,IborIndex,AF47,F47,Volatility,MeanReversion,Permanent,AND(ISERROR(Z47),ISERROR(FuturesHWConvAdj!Q46:Q47)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU2ConvAdj_Quote#0013</v>
+        <v>AUDFUT3MU2ConvAdj_Quote#0001</v>
       </c>
       <c r="AI47" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH47)</f>

</xml_diff>

<commit_message>
AUD standard curve first version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_Market.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15210" windowHeight="8355" tabRatio="723"/>
+    <workbookView minimized="1" xWindow="9585" yWindow="-15" windowWidth="4800" windowHeight="11610" tabRatio="723"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="56" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3099" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="288">
   <si>
     <t>Currency</t>
   </si>
@@ -2999,105 +2999,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 09:08:47</v>
-        <stp/>
-        <stp>{4F080267-A2DE-4034-9BFA-EB6DAF78F6BE}</stp>
-        <tr r="O5" s="17"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:48</v>
-        <stp/>
-        <stp>{9CA386A3-0D90-4B10-B43E-B5E013B1CB43}</stp>
-        <tr r="K5" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:49</v>
-        <stp/>
-        <stp>{9D4D69EB-BD55-424D-A532-DFEA03E8F376}</stp>
-        <tr r="O4" s="22"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:47</v>
-        <stp/>
-        <stp>{770F8C37-CF6C-4EC9-B8CF-EF3A5A700E85}</stp>
-        <tr r="M6" s="7"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:49</v>
-        <stp/>
-        <stp>{55907EA5-63D1-4184-9591-85645854CBE7}</stp>
-        <tr r="N4" s="16"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:48</v>
-        <stp/>
-        <stp>{A509BBFC-EA50-4FD9-8AD0-E0863866154E}</stp>
-        <tr r="P4" s="11"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:49</v>
-        <stp/>
-        <stp>{21D0A4B3-C595-4F9B-8B54-0CF50B9B28ED}</stp>
-        <tr r="O4" s="23"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:48</v>
-        <stp/>
-        <stp>{C38382BD-3D11-42CC-A30D-97D970759534}</stp>
-        <tr r="P4" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:47</v>
-        <stp/>
-        <stp>{F3A5206A-4887-4994-B2C3-A5B7C8A074E2}</stp>
-        <tr r="M6" s="8"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:13:10</v>
-        <stp/>
-        <stp>{353FA217-E300-4313-BC57-C657829F5B3C}</stp>
-        <tr r="O5" s="18"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:49</v>
-        <stp/>
-        <stp>{22154068-A8A9-4A53-B2CF-CB3116AF9B2F}</stp>
-        <tr r="O4" s="65"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:47</v>
-        <stp/>
-        <stp>{98CD1062-EF6E-4EDB-9657-14B19C233D48}</stp>
-        <tr r="J4" s="15"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:48</v>
-        <stp/>
-        <stp>{B891AFD9-0300-43E4-9B9C-A10F353F3AA7}</stp>
-        <tr r="P4" s="25"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:48</v>
-        <stp/>
-        <stp>{0D5B596C-3BEF-4B5B-AD9F-3589E8CE4419}</stp>
-        <tr r="Q5" s="64"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:08:49</v>
-        <stp/>
-        <stp>{086F9DDC-276A-4295-9825-A4F470DA4C81}</stp>
-        <tr r="P4" s="26"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3459,7 +3360,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="266">
-        <v>41809.380694444444</v>
+        <v>41813.401689814818</v>
       </c>
       <c r="E5" s="253"/>
       <c r="G5" s="5"/>
@@ -3496,7 +3397,7 @@
       </c>
       <c r="D7" s="263">
         <f>_xll.ohTrigger(Deposits!R3,FRA!X3,Futures3M!Z4,FuturesHWConvAdj!Q3,Swaps1M!Y3,Swap3M!Z3,Swap6M!Z3,BasisSwap1M3M!X3,BasisSwap3M6M!X3,OIS!Y3)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E7" s="253"/>
       <c r="G7" s="5"/>
@@ -3555,7 +3456,7 @@
       </c>
       <c r="I10" s="397">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41809</v>
+        <v>41813</v>
       </c>
       <c r="J10" s="330"/>
     </row>
@@ -3896,7 +3797,7 @@
       <c r="P3" s="83"/>
       <c r="Q3" s="168">
         <f>_xll.ohTrigger(Q5:Q9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="12"/>
@@ -3989,9 +3890,9 @@
         <f t="array" ref="P5:P6">QuoteLive</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="234">
+      <c r="Q5" s="234" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C5,P5,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="12"/>
@@ -4038,9 +3939,9 @@
       <c r="P6" s="344">
         <v>0.03</v>
       </c>
-      <c r="Q6" s="226">
+      <c r="Q6" s="226" t="e">
         <f>_xll.qlSimpleQuoteSetValue(C6,P6,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R6" s="21"/>
       <c r="S6" s="12"/>
@@ -4258,7 +4159,7 @@
       <c r="X3" s="83"/>
       <c r="Y3" s="168">
         <f>_xll.ohTrigger(Y5:Y15)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="126"/>
     </row>
@@ -4285,9 +4186,9 @@
       <c r="L4" s="115"/>
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
-      <c r="O4" s="134" t="str">
-        <f>_xll.RData(O5:O18,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:08:49</v>
+      <c r="O4" s="134" t="e">
+        <f ca="1">_xll.RData(O5:O18,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P4" s="188" t="s">
         <v>162</v>
@@ -5356,7 +5257,7 @@
       <c r="Y3" s="83"/>
       <c r="Z3" s="168">
         <f>_xll.ohTrigger(Z5:Z42)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="126"/>
       <c r="AB3" s="12"/>
@@ -5391,9 +5292,9 @@
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
       <c r="O4" s="115"/>
-      <c r="P4" s="497" t="str">
-        <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:08:48</v>
+      <c r="P4" s="497" t="e">
+        <f ca="1">_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -5573,9 +5474,9 @@
       <c r="Y6" s="199">
         <v>2.6749999999999998</v>
       </c>
-      <c r="Z6" s="136">
+      <c r="Z6" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F6,Y6/100,Trigger)</f>
-        <v>-9.9999999999999395E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="AA6" s="126"/>
       <c r="AB6" s="12"/>
@@ -5881,9 +5782,9 @@
       <c r="Y10" s="199">
         <v>2.7850000000000001</v>
       </c>
-      <c r="Z10" s="136">
+      <c r="Z10" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F10,Y10/100,Trigger)</f>
-        <v>-3.5000000000000309E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA10" s="126"/>
       <c r="AB10" s="12"/>
@@ -5958,9 +5859,9 @@
       <c r="Y11" s="199">
         <v>2.9349999999999996</v>
       </c>
-      <c r="Z11" s="136">
+      <c r="Z11" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F11,Y11/100,Trigger)</f>
-        <v>-4.750000000000032E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA11" s="126"/>
       <c r="AB11" s="12"/>
@@ -8538,7 +8439,7 @@
       <c r="Y3" s="83"/>
       <c r="Z3" s="168">
         <f>_xll.ohTrigger(Z5:Z42)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="126"/>
       <c r="AB3" s="12"/>
@@ -8572,9 +8473,9 @@
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
       <c r="O4" s="115"/>
-      <c r="P4" s="134" t="str">
-        <f>_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:08:49</v>
+      <c r="P4" s="134" t="e">
+        <f ca="1">_xll.RData(P5:P42,Q4:T4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -9216,9 +9117,9 @@
       <c r="Y12" s="199">
         <v>3.1825000000000001</v>
       </c>
-      <c r="Z12" s="136">
+      <c r="Z12" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F12,Y12/100,Trigger)</f>
-        <v>-5.2500000000000463E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA12" s="126"/>
       <c r="AB12" s="12"/>
@@ -9293,9 +9194,9 @@
       <c r="Y13" s="199">
         <v>3.355</v>
       </c>
-      <c r="Z13" s="136">
+      <c r="Z13" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F13,Y13/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA13" s="126"/>
       <c r="AB13" s="12"/>
@@ -9370,9 +9271,9 @@
       <c r="Y14" s="199">
         <v>3.5274999999999999</v>
       </c>
-      <c r="Z14" s="136">
+      <c r="Z14" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F14,Y14/100,Trigger)</f>
-        <v>-5.2499999999999769E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA14" s="126"/>
       <c r="AB14" s="12"/>
@@ -9447,9 +9348,9 @@
       <c r="Y15" s="199">
         <v>3.6799999999999997</v>
       </c>
-      <c r="Z15" s="136">
+      <c r="Z15" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F15,Y15/100,Trigger)</f>
-        <v>-5.7499999999999912E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA15" s="126"/>
       <c r="AB15" s="12"/>
@@ -9524,9 +9425,9 @@
       <c r="Y16" s="199">
         <v>3.8125</v>
       </c>
-      <c r="Z16" s="136">
+      <c r="Z16" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F16,Y16/100,Trigger)</f>
-        <v>-5.7499999999999912E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA16" s="126"/>
       <c r="AB16" s="12"/>
@@ -9601,9 +9502,9 @@
       <c r="Y17" s="199">
         <v>3.9225000000000003</v>
       </c>
-      <c r="Z17" s="136">
+      <c r="Z17" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F17,Y17/100,Trigger)</f>
-        <v>-5.7499999999999912E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA17" s="126"/>
       <c r="AB17" s="12"/>
@@ -9678,9 +9579,9 @@
       <c r="Y18" s="199">
         <v>4.0199999999999996</v>
       </c>
-      <c r="Z18" s="136">
+      <c r="Z18" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F18,Y18/100,Trigger)</f>
-        <v>-6.0000000000001025E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA18" s="126"/>
       <c r="AB18" s="12"/>
@@ -9832,9 +9733,9 @@
       <c r="Y20" s="199">
         <v>4.18</v>
       </c>
-      <c r="Z20" s="136">
+      <c r="Z20" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20/100,Trigger)</f>
-        <v>-6.0000000000000331E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA20" s="126"/>
       <c r="AB20" s="12"/>
@@ -10063,9 +9964,9 @@
       <c r="Y23" s="199">
         <v>4.33</v>
       </c>
-      <c r="Z23" s="136">
+      <c r="Z23" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F23,Y23/100,Trigger)</f>
-        <v>-5.9999999999999637E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA23" s="126"/>
       <c r="AB23" s="12"/>
@@ -10448,9 +10349,9 @@
       <c r="Y28" s="199">
         <v>4.4474999999999998</v>
       </c>
-      <c r="Z28" s="136">
+      <c r="Z28" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F28,Y28/100,Trigger)</f>
-        <v>-6.0000000000000331E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA28" s="126"/>
       <c r="AB28" s="12"/>
@@ -10833,9 +10734,9 @@
       <c r="Y33" s="199">
         <v>4.4824999999999999</v>
       </c>
-      <c r="Z33" s="136">
+      <c r="Z33" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F33,Y33/100,Trigger)</f>
-        <v>-6.0000000000001025E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA33" s="126"/>
       <c r="AB33" s="12"/>
@@ -11218,9 +11119,9 @@
       <c r="Y38" s="199">
         <v>4.49</v>
       </c>
-      <c r="Z38" s="136">
+      <c r="Z38" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F38,Y38/100,Trigger)</f>
-        <v>-5.9999999999999637E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA38" s="126"/>
       <c r="AB38" s="12"/>
@@ -11372,9 +11273,9 @@
       <c r="Y40" s="199">
         <v>4.45</v>
       </c>
-      <c r="Z40" s="136">
+      <c r="Z40" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F40,Y40/100,Trigger)</f>
-        <v>-5.9999999999999637E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="AA40" s="126"/>
       <c r="AB40" s="12"/>
@@ -11699,7 +11600,7 @@
       <c r="W3" s="83"/>
       <c r="X3" s="168">
         <f>_xll.ohTrigger(X5:X42)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="126"/>
     </row>
@@ -11728,9 +11629,9 @@
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
       <c r="O4" s="115"/>
-      <c r="P4" s="134" t="str">
-        <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:08:48</v>
+      <c r="P4" s="134" t="e">
+        <f ca="1">_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -11816,9 +11717,9 @@
         <f t="array" ref="W5:W42">QuoteLive</f>
         <v>4.75</v>
       </c>
-      <c r="X5" s="136">
+      <c r="X5" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F5,W5/10000,Trigger)</f>
-        <v>2.5000000000000011E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Y5" s="126"/>
       <c r="Z5" s="12"/>
@@ -11888,9 +11789,9 @@
       <c r="W6" s="339">
         <v>5.5</v>
       </c>
-      <c r="X6" s="136">
+      <c r="X6" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y6" s="126"/>
       <c r="Z6" s="12"/>
@@ -12166,9 +12067,9 @@
       <c r="W10" s="339">
         <v>6.5</v>
       </c>
-      <c r="X10" s="136">
+      <c r="X10" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y10" s="126"/>
     </row>
@@ -12233,9 +12134,9 @@
       <c r="W11" s="339">
         <v>6.75</v>
       </c>
-      <c r="X11" s="136">
+      <c r="X11" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y11" s="126"/>
     </row>
@@ -12300,9 +12201,9 @@
       <c r="W12" s="339">
         <v>7.25</v>
       </c>
-      <c r="X12" s="136">
+      <c r="X12" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y12" s="126"/>
     </row>
@@ -12367,9 +12268,9 @@
       <c r="W13" s="339">
         <v>7.5</v>
       </c>
-      <c r="X13" s="136">
+      <c r="X13" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y13" s="126"/>
     </row>
@@ -12501,9 +12402,9 @@
       <c r="W15" s="339">
         <v>7.625</v>
       </c>
-      <c r="X15" s="136">
+      <c r="X15" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y15" s="126"/>
     </row>
@@ -12702,9 +12603,9 @@
       <c r="W18" s="339">
         <v>7.625</v>
       </c>
-      <c r="X18" s="136">
+      <c r="X18" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F18,W18/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y18" s="126"/>
       <c r="AC18"/>
@@ -12837,9 +12738,9 @@
       <c r="W20" s="339">
         <v>7.625</v>
       </c>
-      <c r="X20" s="136">
+      <c r="X20" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F20,W20/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y20" s="126"/>
     </row>
@@ -13038,9 +12939,9 @@
       <c r="W23" s="339">
         <v>7.875</v>
       </c>
-      <c r="X23" s="136">
+      <c r="X23" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F23,W23/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y23" s="126"/>
     </row>
@@ -13373,9 +13274,9 @@
       <c r="W28" s="339">
         <v>7.5</v>
       </c>
-      <c r="X28" s="136">
+      <c r="X28" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F28,W28/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y28" s="126"/>
     </row>
@@ -13708,9 +13609,9 @@
       <c r="W33" s="339">
         <v>6</v>
       </c>
-      <c r="X33" s="136">
+      <c r="X33" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F33,W33/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y33" s="126"/>
     </row>
@@ -14043,9 +13944,9 @@
       <c r="W38" s="339">
         <v>5.75</v>
       </c>
-      <c r="X38" s="136">
+      <c r="X38" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F38,W38/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y38" s="126"/>
     </row>
@@ -14484,7 +14385,7 @@
       <c r="W3" s="83"/>
       <c r="X3" s="168">
         <f>_xll.ohTrigger(X5:X42)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="126"/>
       <c r="Z3" s="12"/>
@@ -14519,9 +14420,9 @@
       <c r="M4" s="115"/>
       <c r="N4" s="115"/>
       <c r="O4" s="115"/>
-      <c r="P4" s="134" t="str">
-        <f>_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
-        <v>Updated at 09:08:48</v>
+      <c r="P4" s="134" t="e">
+        <f ca="1">_xll.RData(P5:P42,Q4:R4,"RTFEED:IDN",ReutersRtMode,,Q5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="Q4" s="188" t="s">
         <v>162</v>
@@ -14612,9 +14513,9 @@
         <f t="array" ref="W5:W42">QuoteLive</f>
         <v>3.625</v>
       </c>
-      <c r="X5" s="136">
+      <c r="X5" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F5,W5/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y5" s="126"/>
       <c r="Z5" s="12"/>
@@ -14683,9 +14584,9 @@
       <c r="W6" s="339">
         <v>5</v>
       </c>
-      <c r="X6" s="136">
+      <c r="X6" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y6" s="126"/>
       <c r="Z6" s="12"/>
@@ -14967,9 +14868,9 @@
       <c r="W10" s="339">
         <v>5.875</v>
       </c>
-      <c r="X10" s="136">
+      <c r="X10" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y10" s="126"/>
       <c r="Z10" s="12"/>
@@ -15038,9 +14939,9 @@
       <c r="W11" s="339">
         <v>6.75</v>
       </c>
-      <c r="X11" s="136">
+      <c r="X11" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y11" s="126"/>
       <c r="Z11" s="12"/>
@@ -15109,9 +15010,9 @@
       <c r="W12" s="339">
         <v>7.125</v>
       </c>
-      <c r="X12" s="136">
+      <c r="X12" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y12" s="126"/>
       <c r="Z12" s="12"/>
@@ -15180,9 +15081,9 @@
       <c r="W13" s="339">
         <v>7.375</v>
       </c>
-      <c r="X13" s="136">
+      <c r="X13" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/10000,Trigger)</f>
-        <v>-1.2500000000000033E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Y13" s="126"/>
       <c r="Z13" s="12"/>
@@ -15322,9 +15223,9 @@
       <c r="W15" s="339">
         <v>7.5</v>
       </c>
-      <c r="X15" s="136">
+      <c r="X15" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y15" s="126"/>
       <c r="Z15" s="12"/>
@@ -15535,9 +15436,9 @@
       <c r="W18" s="339">
         <v>7.5</v>
       </c>
-      <c r="X18" s="136">
+      <c r="X18" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F18,W18/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y18" s="126"/>
       <c r="Z18" s="12"/>
@@ -15677,9 +15578,9 @@
       <c r="W20" s="339">
         <v>7</v>
       </c>
-      <c r="X20" s="136">
+      <c r="X20" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F20,W20/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y20" s="126"/>
       <c r="Z20" s="12"/>
@@ -15890,9 +15791,9 @@
       <c r="W23" s="339">
         <v>6</v>
       </c>
-      <c r="X23" s="136">
+      <c r="X23" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F23,W23/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y23" s="126"/>
       <c r="Z23" s="12"/>
@@ -16245,9 +16146,9 @@
       <c r="W28" s="339">
         <v>4.75</v>
       </c>
-      <c r="X28" s="136">
+      <c r="X28" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F28,W28/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y28" s="126"/>
       <c r="Z28" s="12"/>
@@ -16600,9 +16501,9 @@
       <c r="W33" s="339">
         <v>3.75</v>
       </c>
-      <c r="X33" s="136">
+      <c r="X33" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F33,W33/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y33" s="126"/>
       <c r="Z33" s="12"/>
@@ -16955,9 +16856,9 @@
       <c r="W38" s="339">
         <v>2.75</v>
       </c>
-      <c r="X38" s="136">
+      <c r="X38" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F38,W38/10000,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y38" s="126"/>
       <c r="Z38" s="12"/>
@@ -17462,9 +17363,9 @@
         <v>Error Message LastFixing_Quote</v>
       </c>
       <c r="J5" s="393"/>
-      <c r="K5" s="369" t="str">
-        <f>_xll.RData(K6:K12,L5:M5,"RTFEED:IDN",,,L6)</f>
-        <v>Updated at 09:08:48</v>
+      <c r="K5" s="369" t="e">
+        <f ca="1">_xll.RData(K6:K12,L5:M5,"RTFEED:IDN",,,L6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="L5" s="370" t="s">
         <v>227</v>
@@ -18235,9 +18136,9 @@
       <c r="L6" s="311" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="310" t="str">
-        <f>_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
-        <v>Updated at 09:08:47</v>
+      <c r="M6" s="310" t="e">
+        <f ca="1">_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N6" s="310" t="s">
         <v>227</v>
@@ -20782,9 +20683,9 @@
       <c r="L6" s="311" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="310" t="str">
-        <f>_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
-        <v>Updated at 09:08:47</v>
+      <c r="M6" s="310" t="e">
+        <f ca="1">_xll.RData(M7:M21,N6:O6,"RTFEED:IDN",,,N7)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N6" s="310" t="s">
         <v>227</v>
@@ -23140,7 +23041,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:AA16"/>
+  <dimension ref="B1:AA17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -23155,7 +23056,7 @@
     <col min="7" max="7" width="5" style="384" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" style="384" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="384" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="384" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="384" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="384" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.7109375" style="384" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" style="384" customWidth="1"/>
@@ -23303,9 +23204,9 @@
       <c r="P5" s="369" t="s">
         <v>244</v>
       </c>
-      <c r="Q5" s="370" t="str">
-        <f>_xll.RData(Q6:Q14,R5:S5,"RTFEED:IDN",,,R6)</f>
-        <v>Updated at 09:08:48</v>
+      <c r="Q5" s="370" t="e">
+        <f ca="1">_xll.RData(Q6:Q14,R5:S5,"RTFEED:IDN",,,R6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R5" s="370" t="s">
         <v>227</v>
@@ -23350,25 +23251,25 @@
       </c>
       <c r="J6" s="432" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AUDON#0000</v>
+        <v>AUDON#0001</v>
       </c>
       <c r="K6" s="432" t="str">
         <f>_xll.qlOvernightIndex(I6,,D6,Currency,Calendar,H6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AONIA#0000</v>
+        <v>AONIA#0001</v>
       </c>
       <c r="L6" s="432" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C6&amp;"LastFixing_Quote",K6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWONLastFixing_Quote#0000</v>
+        <v>AudBBSWONLastFixing_Quote#0001</v>
       </c>
       <c r="M6" s="433"/>
       <c r="N6" s="364"/>
       <c r="O6" s="434" t="str">
-        <f t="shared" ref="O6:O14" si="1">C6</f>
+        <f t="shared" ref="O6:O16" si="1">C6</f>
         <v>ON</v>
       </c>
       <c r="P6" s="435" t="str">
         <f>K6</f>
-        <v>AONIA#0000</v>
+        <v>AONIA#0001</v>
       </c>
       <c r="Q6" s="436" t="str">
         <f>"AU"&amp;"CASH"&amp;"="&amp;"RBAA"</f>
@@ -23421,15 +23322,15 @@
       </c>
       <c r="J7" s="363" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AUD1M#0000</v>
+        <v>AUD1M#0001</v>
       </c>
       <c r="K7" s="363" t="str">
         <f>_xll.qlIborIndex(I7,FamilyName,C7,D7,Currency,E7,F7,G7,H7,J7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW1M#0000</v>
+        <v>AudBBSW1M#0001</v>
       </c>
       <c r="L7" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C7&amp;"LastFixing_Quote",K7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW1MLastFixing_Quote#0000</v>
+        <v>AudBBSW1MLastFixing_Quote#0001</v>
       </c>
       <c r="M7" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -23442,7 +23343,7 @@
       </c>
       <c r="P7" s="378" t="str">
         <f>K7</f>
-        <v>AudBBSW1M#0000</v>
+        <v>AudBBSW1M#0001</v>
       </c>
       <c r="Q7" s="376" t="str">
         <f t="shared" ref="Q7:Q13" si="4">"AU"&amp;O7&amp;"BBC"&amp;"="&amp;"ICAA"</f>
@@ -23496,11 +23397,11 @@
       <c r="J8" s="363"/>
       <c r="K8" s="363" t="str">
         <f>_xll.qlIborIndex(I8,FamilyName,C8,D8,Currency,E8,F8,G8,H8,J8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW2M#0000</v>
+        <v>AudBBSW2M#0001</v>
       </c>
       <c r="L8" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C8&amp;"LastFixing_Quote",K8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW2MLastFixing_Quote#0000</v>
+        <v>AudBBSW2MLastFixing_Quote#0001</v>
       </c>
       <c r="M8" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -23513,7 +23414,7 @@
       </c>
       <c r="P8" s="378" t="str">
         <f t="shared" ref="P8:P14" si="5">K8</f>
-        <v>AudBBSW2M#0000</v>
+        <v>AudBBSW2M#0001</v>
       </c>
       <c r="Q8" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23535,7 +23436,7 @@
       </c>
       <c r="V8" s="458">
         <f>_xll.qlQuoteValue(L8)</f>
-        <v>2.69E-2</v>
+        <v>2.6800000000000001E-2</v>
       </c>
       <c r="W8" s="365"/>
     </row>
@@ -23566,15 +23467,15 @@
       </c>
       <c r="J9" s="363" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AUD3M#0000</v>
+        <v>AUD3M#0001</v>
       </c>
       <c r="K9" s="363" t="str">
         <f>_xll.qlIborIndex(I9,FamilyName,C9,D9,Currency,E9,F9,G9,H9,J9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW3M#0000</v>
+        <v>AudBBSW3M#0001</v>
       </c>
       <c r="L9" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C9&amp;"LastFixing_Quote",K9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW3MLastFixing_Quote#0000</v>
+        <v>AudBBSW3MLastFixing_Quote#0001</v>
       </c>
       <c r="M9" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -23587,7 +23488,7 @@
       </c>
       <c r="P9" s="378" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW3M#0000</v>
+        <v>AudBBSW3M#0001</v>
       </c>
       <c r="Q9" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23641,11 +23542,11 @@
       <c r="J10" s="363"/>
       <c r="K10" s="363" t="str">
         <f>_xll.qlIborIndex(I10,FamilyName,C10,D10,Currency,E10,F10,G10,H10,J10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW4M#0000</v>
+        <v>AudBBSW4M#0001</v>
       </c>
       <c r="L10" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C10&amp;"LastFixing_Quote",K10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW4MLastFixing_Quote#0000</v>
+        <v>AudBBSW4MLastFixing_Quote#0001</v>
       </c>
       <c r="M10" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -23658,7 +23559,7 @@
       </c>
       <c r="P10" s="378" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW4M#0000</v>
+        <v>AudBBSW4M#0001</v>
       </c>
       <c r="Q10" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23712,11 +23613,11 @@
       <c r="J11" s="363"/>
       <c r="K11" s="363" t="str">
         <f>_xll.qlIborIndex(I11,FamilyName,C11,D11,Currency,E11,F11,G11,H11,J11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW5M#0000</v>
+        <v>AudBBSW5M#0001</v>
       </c>
       <c r="L11" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C11&amp;"LastFixing_Quote",K11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW5MLastFixing_Quote#0000</v>
+        <v>AudBBSW5MLastFixing_Quote#0001</v>
       </c>
       <c r="M11" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K11)</f>
@@ -23729,7 +23630,7 @@
       </c>
       <c r="P11" s="378" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW5M#0000</v>
+        <v>AudBBSW5M#0001</v>
       </c>
       <c r="Q11" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23782,15 +23683,15 @@
       </c>
       <c r="J12" s="363" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AUD6M#0000</v>
+        <v>AUD6M#0001</v>
       </c>
       <c r="K12" s="363" t="str">
         <f>_xll.qlIborIndex(I12,FamilyName,C12,D12,Currency,E12,F12,G12,H12,J12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW6M#0000</v>
+        <v>AudBBSW6M#0001</v>
       </c>
       <c r="L12" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C12&amp;"LastFixing_Quote",K12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW6MLastFixing_Quote#0000</v>
+        <v>AudBBSW6MLastFixing_Quote#0001</v>
       </c>
       <c r="M12" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K12)</f>
@@ -23803,7 +23704,7 @@
       </c>
       <c r="P12" s="378" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW6M#0000</v>
+        <v>AudBBSW6M#0001</v>
       </c>
       <c r="Q12" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23825,7 +23726,7 @@
       </c>
       <c r="V12" s="458">
         <f>_xll.qlQuoteValue(L12)</f>
-        <v>2.7099999999999999E-2</v>
+        <v>2.7200000000000002E-2</v>
       </c>
       <c r="W12" s="365"/>
     </row>
@@ -23857,11 +23758,11 @@
       <c r="J13" s="363"/>
       <c r="K13" s="363" t="str">
         <f>_xll.qlIborIndex(I13,FamilyName,C13,D13,Currency,E13,F13,G13,H13,J13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW9M#0000</v>
+        <v>AudBBSW9M#0001</v>
       </c>
       <c r="L13" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C13&amp;"LastFixing_Quote",K13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW9MLastFixing_Quote#0000</v>
+        <v>AudBBSW9MLastFixing_Quote#0001</v>
       </c>
       <c r="M13" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K13)</f>
@@ -23874,7 +23775,7 @@
       </c>
       <c r="P13" s="378" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW9M#0000</v>
+        <v>AudBBSW9M#0001</v>
       </c>
       <c r="Q13" s="376" t="str">
         <f t="shared" si="4"/>
@@ -23928,11 +23829,11 @@
       <c r="J14" s="363"/>
       <c r="K14" s="363" t="str">
         <f>_xll.qlIborIndex(I14,FamilyName,C14,D14,Currency,E14,F14,G14,H14,J14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW1Y#0000</v>
+        <v>AudBBSW1Y#0001</v>
       </c>
       <c r="L14" s="363" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C14&amp;"LastFixing_Quote",K14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSW1YLastFixing_Quote#0000</v>
+        <v>AudBBSW1YLastFixing_Quote#0001</v>
       </c>
       <c r="M14" s="363" t="str">
         <f>_xll.ohRangeRetrieveError(K14)</f>
@@ -23945,7 +23846,7 @@
       </c>
       <c r="P14" s="415" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW1Y#0000</v>
+        <v>AudBBSW1Y#0001</v>
       </c>
       <c r="Q14" s="416" t="str">
         <f>"AU"&amp;O14&amp;"BBC"&amp;"="&amp;"ICAA"</f>
@@ -23971,44 +23872,73 @@
       </c>
       <c r="W14" s="365"/>
     </row>
-    <row r="15" spans="2:27" s="355" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="381"/>
-      <c r="C15" s="382"/>
-      <c r="D15" s="382"/>
-      <c r="E15" s="382"/>
-      <c r="F15" s="382"/>
-      <c r="G15" s="382"/>
-      <c r="H15" s="382"/>
-      <c r="I15" s="382"/>
-      <c r="J15" s="382"/>
-      <c r="K15" s="382"/>
-      <c r="L15" s="382"/>
-      <c r="M15" s="382"/>
-      <c r="N15" s="382"/>
-      <c r="O15" s="382"/>
-      <c r="P15" s="382"/>
-      <c r="Q15" s="382"/>
-      <c r="R15" s="382"/>
-      <c r="S15" s="382"/>
-      <c r="T15" s="382"/>
-      <c r="U15" s="382"/>
-      <c r="V15" s="382"/>
-      <c r="W15" s="383"/>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="355"/>
-      <c r="C16" s="355"/>
-      <c r="D16" s="355"/>
-      <c r="Q16" s="355"/>
-      <c r="R16" s="355"/>
-      <c r="T16" s="355"/>
-      <c r="U16" s="355"/>
-      <c r="V16" s="355"/>
-      <c r="W16" s="355"/>
+    <row r="15" spans="2:27" s="355" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="360"/>
+      <c r="C15" s="372" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="414"/>
+      <c r="E15" s="414"/>
+      <c r="F15" s="419"/>
+      <c r="G15" s="414"/>
+      <c r="H15" s="414"/>
+      <c r="I15" s="414"/>
+      <c r="J15" s="363" t="str">
+        <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C15,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>AUDSTD#0004</v>
+      </c>
+      <c r="K15" s="363"/>
+      <c r="L15" s="363"/>
+      <c r="M15" s="363"/>
+      <c r="N15" s="364"/>
+      <c r="O15" s="361"/>
+      <c r="P15" s="361"/>
+      <c r="Q15" s="361"/>
+      <c r="R15" s="361"/>
+      <c r="S15" s="361"/>
+      <c r="T15" s="361"/>
+      <c r="U15" s="361"/>
+      <c r="V15" s="361"/>
+      <c r="W15" s="365"/>
+    </row>
+    <row r="16" spans="2:27" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="381"/>
+      <c r="C16" s="382"/>
+      <c r="D16" s="382"/>
+      <c r="E16" s="382"/>
+      <c r="F16" s="382"/>
+      <c r="G16" s="382"/>
+      <c r="H16" s="382"/>
+      <c r="I16" s="382"/>
+      <c r="J16" s="382"/>
+      <c r="K16" s="382"/>
+      <c r="L16" s="382"/>
+      <c r="M16" s="382"/>
+      <c r="N16" s="382"/>
+      <c r="O16" s="382"/>
+      <c r="P16" s="382"/>
+      <c r="Q16" s="382"/>
+      <c r="R16" s="382"/>
+      <c r="S16" s="382"/>
+      <c r="T16" s="382"/>
+      <c r="U16" s="382"/>
+      <c r="V16" s="382"/>
+      <c r="W16" s="383"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B17" s="355"/>
+      <c r="C17" s="355"/>
+      <c r="D17" s="355"/>
+      <c r="Q17" s="355"/>
+      <c r="R17" s="355"/>
+      <c r="T17" s="355"/>
+      <c r="U17" s="355"/>
+      <c r="V17" s="355"/>
+      <c r="W17" s="355"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H15">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -24084,7 +24014,7 @@
       </c>
       <c r="F4" s="406" t="str">
         <f>_xll.qlSwapIndex($E4,FixingType,C4,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWSwapForBasisCalc1Y#0000</v>
+        <v>AudBBSWSwapForBasisCalc1Y#0003</v>
       </c>
       <c r="G4" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -24106,7 +24036,7 @@
       </c>
       <c r="F5" s="406" t="str">
         <f>_xll.qlSwapIndex($E5,FixingType,C5,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWSwapForBasisCalc2Y#0000</v>
+        <v>AudBBSWSwapForBasisCalc2Y#0003</v>
       </c>
       <c r="G5" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -24128,7 +24058,7 @@
       </c>
       <c r="F6" s="406" t="str">
         <f>_xll.qlSwapIndex($E6,FixingType,C6,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWSwapForBasisCalc3Y#0000</v>
+        <v>AudBBSWSwapForBasisCalc3Y#0003</v>
       </c>
       <c r="G6" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -24150,7 +24080,7 @@
       </c>
       <c r="F7" s="406" t="str">
         <f>_xll.qlSwapIndex($E7,FixingType,C7,1,Currency,Calendar,"3M","mf","act/365 (fixed)",BBSW!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>AudBBSWSwapForBasisCalc4Y#0000</v>
+        <v>AudBBSWSwapForBasisCalc4Y#0003</v>
       </c>
       <c r="G7" s="403" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -24849,7 +24779,7 @@
       <c r="X3" s="83"/>
       <c r="Y3" s="168">
         <f>_xll.ohTrigger(Y5:Y24)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="126"/>
     </row>
@@ -24876,9 +24806,9 @@
       <c r="L4" s="82"/>
       <c r="M4" s="82"/>
       <c r="N4" s="82"/>
-      <c r="O4" s="220" t="str">
-        <f>_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:08:49</v>
+      <c r="O4" s="220" t="e">
+        <f ca="1">_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P4" s="217" t="s">
         <v>162</v>
@@ -24971,9 +24901,9 @@
         <f t="array" ref="X5:X58">QuoteLive</f>
         <v>2.5</v>
       </c>
-      <c r="Y5" s="155">
+      <c r="Y5" s="155" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F5,X5/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Z5" s="126"/>
     </row>
@@ -25172,9 +25102,9 @@
       <c r="X8" s="199">
         <v>2.4990000000000001</v>
       </c>
-      <c r="Y8" s="136">
+      <c r="Y8" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F8,X8/100,Trigger)</f>
-        <v>-9.9999999999995925E-6</v>
+        <v>#N/A</v>
       </c>
       <c r="Z8" s="126"/>
       <c r="AB8"/>
@@ -25240,9 +25170,9 @@
       <c r="X9" s="199">
         <v>2.4975000000000001</v>
       </c>
-      <c r="Y9" s="136">
+      <c r="Y9" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F9,X9/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Z9" s="126"/>
     </row>
@@ -25307,9 +25237,9 @@
       <c r="X10" s="199">
         <v>2.4950000000000001</v>
       </c>
-      <c r="Y10" s="136">
+      <c r="Y10" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F10,X10/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Z10" s="126"/>
     </row>
@@ -25374,9 +25304,9 @@
       <c r="X11" s="199">
         <v>2.4925000000000002</v>
       </c>
-      <c r="Y11" s="136">
+      <c r="Y11" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
-        <v>-9.9999999999961231E-6</v>
+        <v>#N/A</v>
       </c>
       <c r="Z11" s="126"/>
     </row>
@@ -25441,9 +25371,9 @@
       <c r="X12" s="199">
         <v>2.4925000000000002</v>
       </c>
-      <c r="Y12" s="136">
+      <c r="Y12" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Z12" s="126"/>
     </row>
@@ -25508,9 +25438,9 @@
       <c r="X13" s="199">
         <v>2.4910000000000001</v>
       </c>
-      <c r="Y13" s="136">
+      <c r="Y13" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F13,X13/100,Trigger)</f>
-        <v>-1.5000000000001124E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Z13" s="126"/>
     </row>
@@ -25709,9 +25639,9 @@
       <c r="X16" s="199">
         <v>2.4900000000000002</v>
       </c>
-      <c r="Y16" s="136">
+      <c r="Y16" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F16,X16/100,Trigger)</f>
-        <v>-9.9999999999999395E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Z16" s="126"/>
     </row>
@@ -25910,9 +25840,9 @@
       <c r="X19" s="199">
         <v>2.5009999999999999</v>
       </c>
-      <c r="Y19" s="136">
+      <c r="Y19" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F19,X19/100,Trigger)</f>
-        <v>-2.2499999999999951E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z19" s="126"/>
     </row>
@@ -26312,9 +26242,9 @@
       <c r="X25" s="199">
         <v>2.5649999999999999</v>
       </c>
-      <c r="Y25" s="136">
+      <c r="Y25" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F25,X25/100,Trigger)</f>
-        <v>-2.9999999999999818E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z25" s="126"/>
     </row>
@@ -26714,9 +26644,9 @@
       <c r="X31" s="199">
         <v>2.65</v>
       </c>
-      <c r="Y31" s="136">
+      <c r="Y31" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F31,X31/100,Trigger)</f>
-        <v>-4.0000000000000105E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z31" s="126"/>
     </row>
@@ -26982,9 +26912,9 @@
       <c r="X35" s="199">
         <v>2.855</v>
       </c>
-      <c r="Y35" s="136">
+      <c r="Y35" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F35,X35/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z35" s="126"/>
     </row>
@@ -28803,7 +28733,7 @@
       <c r="X3" s="83"/>
       <c r="Y3" s="168">
         <f>_xll.ohTrigger(Y5:Y24)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="126"/>
     </row>
@@ -28830,9 +28760,9 @@
       <c r="L4" s="82"/>
       <c r="M4" s="82"/>
       <c r="N4" s="82"/>
-      <c r="O4" s="220" t="str">
-        <f>_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
-        <v>Updated at 09:08:49</v>
+      <c r="O4" s="220" t="e">
+        <f ca="1">_xll.RData(O5:O58,P4:S4,"RTFEED:IDN",ReutersRtMode,,P5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P4" s="217" t="s">
         <v>162</v>
@@ -29923,9 +29853,9 @@
       <c r="X19" s="199">
         <v>2.508</v>
       </c>
-      <c r="Y19" s="136">
+      <c r="Y19" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F19,X19/100,Trigger)</f>
-        <v>-1.6999999999999654E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z19" s="126"/>
     </row>
@@ -30349,9 +30279,9 @@
       <c r="X25" s="199">
         <v>2.5449999999999999</v>
       </c>
-      <c r="Y25" s="136">
+      <c r="Y25" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F25,X25/100,Trigger)</f>
-        <v>-3.0000000000000165E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z25" s="126"/>
     </row>
@@ -30775,9 +30705,9 @@
       <c r="X31" s="199">
         <v>2.62</v>
       </c>
-      <c r="Y31" s="136">
+      <c r="Y31" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F31,X31/100,Trigger)</f>
-        <v>-3.5000000000000309E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z31" s="126"/>
     </row>
@@ -31059,9 +30989,9 @@
       <c r="X35" s="199">
         <v>2.7749999999999999</v>
       </c>
-      <c r="Y35" s="136">
+      <c r="Y35" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F35,X35/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z35" s="126"/>
     </row>
@@ -31343,9 +31273,9 @@
       <c r="X39" s="199">
         <v>2.92</v>
       </c>
-      <c r="Y39" s="136">
+      <c r="Y39" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F39,X39/100,Trigger)</f>
-        <v>-5.2999999999999922E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z39" s="126"/>
     </row>
@@ -31627,9 +31557,9 @@
       <c r="X43" s="199">
         <v>3.0780000000000003</v>
       </c>
-      <c r="Y43" s="136">
+      <c r="Y43" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F43,X43/100,Trigger)</f>
-        <v>-5.4999999999999494E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z43" s="126"/>
     </row>
@@ -31698,9 +31628,9 @@
       <c r="X44" s="199">
         <v>3.238</v>
       </c>
-      <c r="Y44" s="136">
+      <c r="Y44" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F44,X44/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z44" s="126"/>
     </row>
@@ -31769,9 +31699,9 @@
       <c r="X45" s="199">
         <v>3.3980000000000001</v>
       </c>
-      <c r="Y45" s="136">
+      <c r="Y45" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F45,X45/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z45" s="126"/>
     </row>
@@ -31840,9 +31770,9 @@
       <c r="X46" s="199">
         <v>3.5049999999999999</v>
       </c>
-      <c r="Y46" s="136">
+      <c r="Y46" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>-5.5000000000000188E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z46" s="126"/>
     </row>
@@ -31911,9 +31841,9 @@
       <c r="X47" s="199">
         <v>3.61</v>
       </c>
-      <c r="Y47" s="136">
+      <c r="Y47" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>-5.9999999999999637E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z47" s="126"/>
     </row>
@@ -31982,9 +31912,9 @@
       <c r="X48" s="199">
         <v>3.718</v>
       </c>
-      <c r="Y48" s="136">
+      <c r="Y48" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>-6.0000000000000331E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z48" s="126"/>
     </row>
@@ -32053,9 +31983,9 @@
       <c r="X49" s="199">
         <v>3.8650000000000002</v>
       </c>
-      <c r="Y49" s="136">
+      <c r="Y49" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>-6.2999999999999862E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z49" s="126"/>
     </row>
@@ -32124,9 +32054,9 @@
       <c r="X50" s="199">
         <v>4.008</v>
       </c>
-      <c r="Y50" s="136">
+      <c r="Y50" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>-5.9999999999999637E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z50" s="126"/>
     </row>
@@ -32195,9 +32125,9 @@
       <c r="X51" s="199">
         <v>4.1379999999999999</v>
       </c>
-      <c r="Y51" s="136">
+      <c r="Y51" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>-6.0000000000000331E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z51" s="126"/>
     </row>
@@ -32266,9 +32196,9 @@
       <c r="X52" s="199">
         <v>4.1929999999999996</v>
       </c>
-      <c r="Y52" s="136">
+      <c r="Y52" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>-6.0000000000000331E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z52" s="126"/>
     </row>
@@ -32408,9 +32338,9 @@
       <c r="X54" s="199">
         <v>4.2149999999999999</v>
       </c>
-      <c r="Y54" s="136">
+      <c r="Y54" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>-6.3000000000000556E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Z54" s="126"/>
     </row>
@@ -32861,7 +32791,9 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -32962,7 +32894,7 @@
       <c r="Q3" s="169"/>
       <c r="R3" s="168">
         <f>_xll.ohTrigger(R5:R18)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S3" s="126"/>
       <c r="T3" s="12"/>
@@ -32990,9 +32922,9 @@
       <c r="F4" s="126"/>
       <c r="H4" s="80"/>
       <c r="I4" s="165"/>
-      <c r="J4" s="134" t="str">
-        <f>_xll.RData(J6:J22,K4:L4,,ReutersRtMode,,K6)</f>
-        <v>Updated at 09:08:47</v>
+      <c r="J4" s="134" t="e">
+        <f ca="1">_xll.RData(J6:J22,K4:L4,,ReutersRtMode,,K6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="K4" s="134" t="s">
         <v>162</v>
@@ -34344,7 +34276,7 @@
       <c r="W3" s="83"/>
       <c r="X3" s="168">
         <f>_xll.ohTrigger(X5:X19)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="126"/>
       <c r="Z3" s="12"/>
@@ -34369,9 +34301,9 @@
       <c r="K4" s="115"/>
       <c r="L4" s="91"/>
       <c r="M4" s="59"/>
-      <c r="N4" s="473" t="str">
-        <f>_xll.RData(N5:N19,O4:R4,"RTFEED:IDN",ReutersRtMode,,O5)</f>
-        <v>Updated at 09:08:49</v>
+      <c r="N4" s="473" t="e">
+        <f ca="1">_xll.RData(N5:N19,O4:R4,"RTFEED:IDN",ReutersRtMode,,O5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="O4" s="166" t="s">
         <v>162</v>
@@ -34469,9 +34401,9 @@
         <f t="array" ref="W5:W19">QuoteLive</f>
         <v>2.7</v>
       </c>
-      <c r="X5" s="155">
+      <c r="X5" s="155" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E5,W5/100,Trigger)</f>
-        <v>1.500000000000043E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y5" s="126"/>
       <c r="Z5" s="12"/>
@@ -34541,9 +34473,9 @@
       <c r="W6" s="199">
         <v>2.665</v>
       </c>
-      <c r="X6" s="136">
+      <c r="X6" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E6,W6/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y6" s="126"/>
       <c r="Z6" s="12"/>
@@ -34613,9 +34545,9 @@
       <c r="W7" s="199">
         <v>2.6550000000000002</v>
       </c>
-      <c r="X7" s="136">
+      <c r="X7" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E7,W7/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y7" s="126"/>
       <c r="Z7" s="12"/>
@@ -34685,9 +34617,9 @@
       <c r="W8" s="199">
         <v>2.645</v>
       </c>
-      <c r="X8" s="136">
+      <c r="X8" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E8,W8/100,Trigger)</f>
-        <v>-1.0000000000000286E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y8" s="126"/>
       <c r="Z8" s="12"/>
@@ -34757,9 +34689,9 @@
       <c r="W9" s="199">
         <v>2.645</v>
       </c>
-      <c r="X9" s="136">
+      <c r="X9" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E9,W9/100,Trigger)</f>
-        <v>-1.0000000000000286E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y9" s="126"/>
       <c r="Z9" s="12"/>
@@ -34829,9 +34761,9 @@
       <c r="W10" s="199">
         <v>2.645</v>
       </c>
-      <c r="X10" s="136">
+      <c r="X10" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E10,W10/100,Trigger)</f>
-        <v>-2.4999999999999675E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y10" s="126"/>
       <c r="Z10" s="12"/>
@@ -34902,9 +34834,9 @@
       <c r="W11" s="476">
         <v>2.69</v>
       </c>
-      <c r="X11" s="477">
+      <c r="X11" s="477" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E11,W11/100,Trigger)</f>
-        <v>9.9999999999999395E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Y11" s="126"/>
       <c r="Z11" s="12"/>
@@ -34975,9 +34907,9 @@
       <c r="W12" s="199">
         <v>2.68</v>
       </c>
-      <c r="X12" s="136">
+      <c r="X12" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E12,W12/100,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="Y12" s="126"/>
       <c r="Z12" s="12"/>
@@ -35048,9 +34980,9 @@
       <c r="W13" s="199">
         <v>2.67</v>
       </c>
-      <c r="X13" s="136">
+      <c r="X13" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E13,W13/100,Trigger)</f>
-        <v>-1.0000000000000286E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y13" s="126"/>
       <c r="Z13" s="12"/>
@@ -35121,9 +35053,9 @@
       <c r="W14" s="199">
         <v>2.67</v>
       </c>
-      <c r="X14" s="136">
+      <c r="X14" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E14,W14/100,Trigger)</f>
-        <v>-1.0000000000000286E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y14" s="126"/>
       <c r="Z14" s="12"/>
@@ -35194,9 +35126,9 @@
       <c r="W15" s="199">
         <v>2.68</v>
       </c>
-      <c r="X15" s="136">
+      <c r="X15" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E15,W15/100,Trigger)</f>
-        <v>-9.9999999999999395E-5</v>
+        <v>#N/A</v>
       </c>
       <c r="Y15" s="126"/>
       <c r="Z15" s="12"/>
@@ -35267,9 +35199,9 @@
       <c r="W16" s="199">
         <v>2.68</v>
       </c>
-      <c r="X16" s="136">
+      <c r="X16" s="136" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E16,W16/100,Trigger)</f>
-        <v>-2.0000000000000226E-4</v>
+        <v>#N/A</v>
       </c>
       <c r="Y16" s="126"/>
       <c r="Z16" s="12"/>
@@ -35734,7 +35666,7 @@
       <c r="Y4" s="83"/>
       <c r="Z4" s="168">
         <f>_xll.ohTrigger(Z6:Z17)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="213"/>
       <c r="AB4" s="12"/>
@@ -35792,9 +35724,9 @@
       <c r="N5" s="188" t="s">
         <v>196</v>
       </c>
-      <c r="O5" s="134" t="str">
-        <f>_xll.RData(O6:O17,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
-        <v>Updated at 09:08:47</v>
+      <c r="O5" s="134" t="e">
+        <f ca="1">_xll.RData(O6:O17,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P5" s="188" t="s">
         <v>195</v>
@@ -37381,7 +37313,7 @@
       <c r="Y4" s="83"/>
       <c r="Z4" s="168">
         <f>_xll.ohTrigger(Z6:Z47)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="213"/>
       <c r="AB4" s="12"/>
@@ -37394,7 +37326,7 @@
       </c>
       <c r="AH4" s="132" t="str">
         <f>BBSW!K9</f>
-        <v>AudBBSW3M#0000</v>
+        <v>AudBBSW3M#0001</v>
       </c>
       <c r="AI4" s="131" t="s">
         <v>17</v>
@@ -37438,9 +37370,9 @@
       <c r="N5" s="217" t="s">
         <v>196</v>
       </c>
-      <c r="O5" s="220" t="str">
-        <f>_xll.RData(O6:O47,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
-        <v>Updated at 09:13:10</v>
+      <c r="O5" s="220" t="e">
+        <f ca="1">_xll.RData(O6:O47,P5:T5,"RTFEED:IDN",ReutersRtMode,,P6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="P5" s="217" t="s">
         <v>195</v>
@@ -37592,7 +37524,7 @@
       </c>
       <c r="AH6" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG6,IborIndex,AF6,F6,Volatility,MeanReversion,Permanent,AND(ISERROR(Z6),ISERROR(FuturesHWConvAdj!Q5:Q6)),ObjectOverwrite)</f>
-        <v>AUDFUT3MN4ConvAdj_Quote#0007</v>
+        <v>AUDFUT3MN4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI6" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH6)</f>
@@ -37689,7 +37621,7 @@
       </c>
       <c r="AH7" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG7,IborIndex,AF7,F7,Volatility,MeanReversion,Permanent,AND(ISERROR(Z7),ISERROR(FuturesHWConvAdj!Q6:Q7)),ObjectOverwrite)</f>
-        <v>AUDFUT3MQ4ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MQ4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI7" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH7)</f>
@@ -37764,9 +37696,9 @@
       <c r="Y8" s="199">
         <v>97.34</v>
       </c>
-      <c r="Z8" s="141">
+      <c r="Z8" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F8,Y8,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA8" s="21"/>
       <c r="AB8" s="12"/>
@@ -37786,7 +37718,7 @@
       </c>
       <c r="AH8" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG8,IborIndex,AF8,F8,Volatility,MeanReversion,Permanent,AND(ISERROR(Z8),ISERROR(FuturesHWConvAdj!Q7:Q8)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU4ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI8" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH8)</f>
@@ -37883,7 +37815,7 @@
       </c>
       <c r="AH9" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG9,IborIndex,AF9,F9,Volatility,MeanReversion,Permanent,AND(ISERROR(Z9),ISERROR(FuturesHWConvAdj!Q8:Q9)),ObjectOverwrite)</f>
-        <v>AUDFUT3MV4ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MV4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI9" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH9)</f>
@@ -37981,7 +37913,7 @@
       </c>
       <c r="AH10" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG10,IborIndex,AF10,F10,Volatility,MeanReversion,Permanent,AND(ISERROR(Z10),ISERROR(FuturesHWConvAdj!Q9:Q10)),ObjectOverwrite)</f>
-        <v>AUDFUT3MX4ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MX4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI10" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH10)</f>
@@ -38056,9 +37988,9 @@
       <c r="Y11" s="199">
         <v>97.35</v>
       </c>
-      <c r="Z11" s="141">
+      <c r="Z11" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F11,Y11,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA11" s="21"/>
       <c r="AB11" s="12"/>
@@ -38078,7 +38010,7 @@
       </c>
       <c r="AH11" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG11,IborIndex,AF11,F11,Volatility,MeanReversion,Permanent,AND(ISERROR(Z11),ISERROR(FuturesHWConvAdj!Q10:Q11)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ4ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ4ConvAdj_Quote#0003</v>
       </c>
       <c r="AI11" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH11)</f>
@@ -38175,7 +38107,7 @@
       </c>
       <c r="AH12" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG12,IborIndex,AF12,F12,Volatility,MeanReversion,Permanent,AND(ISERROR(Z12),ISERROR(FuturesHWConvAdj!Q11:Q12)),ObjectOverwrite)</f>
-        <v>AUDFUT3MF5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MF5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI12" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH12)</f>
@@ -38272,7 +38204,7 @@
       </c>
       <c r="AH13" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG13,IborIndex,AF13,F13,Volatility,MeanReversion,Permanent,AND(ISERROR(Z13),ISERROR(FuturesHWConvAdj!Q12:Q13)),ObjectOverwrite)</f>
-        <v>AUDFUT3MG5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MG5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI13" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH13)</f>
@@ -38347,9 +38279,9 @@
       <c r="Y14" s="199">
         <v>97.33</v>
       </c>
-      <c r="Z14" s="141">
+      <c r="Z14" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F14,Y14,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA14" s="21"/>
       <c r="AB14" s="12"/>
@@ -38369,7 +38301,7 @@
       </c>
       <c r="AH14" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG14,IborIndex,AF14,F14,Volatility,MeanReversion,Permanent,AND(ISERROR(Z14),ISERROR(FuturesHWConvAdj!Q13:Q14)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI14" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH14)</f>
@@ -38466,7 +38398,7 @@
       </c>
       <c r="AH15" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG15,IborIndex,AF15,F15,Volatility,MeanReversion,Permanent,AND(ISERROR(Z15),ISERROR(FuturesHWConvAdj!Q14:Q15)),ObjectOverwrite)</f>
-        <v>AUDFUT3MJ5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MJ5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI15" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH15)</f>
@@ -38563,7 +38495,7 @@
       </c>
       <c r="AH16" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG16,IborIndex,AF16,F16,Volatility,MeanReversion,Permanent,AND(ISERROR(Z16),ISERROR(FuturesHWConvAdj!Q15:Q16)),ObjectOverwrite)</f>
-        <v>AUDFUT3MK5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MK5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI16" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH16)</f>
@@ -38638,9 +38570,9 @@
       <c r="Y17" s="199">
         <v>97.25</v>
       </c>
-      <c r="Z17" s="141">
+      <c r="Z17" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F17,Y17,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA17" s="21"/>
       <c r="AB17" s="12"/>
@@ -38660,7 +38592,7 @@
       </c>
       <c r="AH17" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG17,IborIndex,AF17,F17,Volatility,MeanReversion,Permanent,AND(ISERROR(Z17),ISERROR(FuturesHWConvAdj!Q16:Q17)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI17" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH17)</f>
@@ -38735,9 +38667,9 @@
       <c r="Y18" s="199">
         <v>97.16</v>
       </c>
-      <c r="Z18" s="141">
+      <c r="Z18" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F18,Y18,Trigger)</f>
-        <v>4.9999999999954525E-3</v>
+        <v>#N/A</v>
       </c>
       <c r="AA18" s="21"/>
       <c r="AB18" s="12"/>
@@ -38757,7 +38689,7 @@
       </c>
       <c r="AH18" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG18,IborIndex,AF18,F18,Volatility,MeanReversion,Permanent,AND(ISERROR(Z18),ISERROR(FuturesHWConvAdj!Q17:Q18)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI18" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH18)</f>
@@ -38832,9 +38764,9 @@
       <c r="Y19" s="199">
         <v>97.06</v>
       </c>
-      <c r="Z19" s="141">
+      <c r="Z19" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F19,Y19,Trigger)</f>
-        <v>4.9999999999954525E-3</v>
+        <v>#N/A</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="12"/>
@@ -38854,7 +38786,7 @@
       </c>
       <c r="AH19" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG19,IborIndex,AF19,F19,Volatility,MeanReversion,Permanent,AND(ISERROR(Z19),ISERROR(FuturesHWConvAdj!Q18:Q19)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ5ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ5ConvAdj_Quote#0003</v>
       </c>
       <c r="AI19" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH19)</f>
@@ -38929,9 +38861,9 @@
       <c r="Y20" s="199">
         <v>96.954999999999998</v>
       </c>
-      <c r="Z20" s="141">
+      <c r="Z20" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F20,Y20,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA20" s="21"/>
       <c r="AB20" s="12"/>
@@ -38951,7 +38883,7 @@
       </c>
       <c r="AH20" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG20,IborIndex,AF20,F20,Volatility,MeanReversion,Permanent,AND(ISERROR(Z20),ISERROR(FuturesHWConvAdj!Q19:Q20)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH6ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH6ConvAdj_Quote#0003</v>
       </c>
       <c r="AI20" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH20)</f>
@@ -39026,9 +38958,9 @@
       <c r="Y21" s="199">
         <v>96.85499999999999</v>
       </c>
-      <c r="Z21" s="141">
+      <c r="Z21" s="141" t="e">
         <f>_xll.qlSimpleQuoteSetValue(F21,Y21,Trigger)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA21" s="21"/>
       <c r="AB21" s="12"/>
@@ -39048,7 +38980,7 @@
       </c>
       <c r="AH21" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG21,IborIndex,AF21,F21,Volatility,MeanReversion,Permanent,AND(ISERROR(Z21),ISERROR(FuturesHWConvAdj!Q20:Q21)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM6ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM6ConvAdj_Quote#0003</v>
       </c>
       <c r="AI21" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH21)</f>
@@ -39145,7 +39077,7 @@
       </c>
       <c r="AH22" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG22,IborIndex,AF22,F22,Volatility,MeanReversion,Permanent,AND(ISERROR(Z22),ISERROR(FuturesHWConvAdj!Q21:Q22)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU6ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU6ConvAdj_Quote#0003</v>
       </c>
       <c r="AI22" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH22)</f>
@@ -39242,7 +39174,7 @@
       </c>
       <c r="AH23" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG23,IborIndex,AF23,F23,Volatility,MeanReversion,Permanent,AND(ISERROR(Z23),ISERROR(FuturesHWConvAdj!Q22:Q23)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ6ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ6ConvAdj_Quote#0003</v>
       </c>
       <c r="AI23" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH23)</f>
@@ -39339,7 +39271,7 @@
       </c>
       <c r="AH24" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG24,IborIndex,AF24,F24,Volatility,MeanReversion,Permanent,AND(ISERROR(Z24),ISERROR(FuturesHWConvAdj!Q23:Q24)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH7ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH7ConvAdj_Quote#0003</v>
       </c>
       <c r="AI24" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH24)</f>
@@ -39436,7 +39368,7 @@
       </c>
       <c r="AH25" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG25,IborIndex,AF25,F25,Volatility,MeanReversion,Permanent,AND(ISERROR(Z25),ISERROR(FuturesHWConvAdj!Q24:Q25)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM7ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM7ConvAdj_Quote#0003</v>
       </c>
       <c r="AI25" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH25)</f>
@@ -39533,7 +39465,7 @@
       </c>
       <c r="AH26" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG26,IborIndex,AF26,F26,Volatility,MeanReversion,Permanent,AND(ISERROR(Z26),ISERROR(FuturesHWConvAdj!Q25:Q26)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU7ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU7ConvAdj_Quote#0003</v>
       </c>
       <c r="AI26" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH26)</f>
@@ -39630,7 +39562,7 @@
       </c>
       <c r="AH27" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG27,IborIndex,AF27,F27,Volatility,MeanReversion,Permanent,AND(ISERROR(Z27),ISERROR(FuturesHWConvAdj!Q26:Q27)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ7ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ7ConvAdj_Quote#0003</v>
       </c>
       <c r="AI27" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH27)</f>
@@ -39727,7 +39659,7 @@
       </c>
       <c r="AH28" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG28,IborIndex,AF28,F28,Volatility,MeanReversion,Permanent,AND(ISERROR(Z28),ISERROR(FuturesHWConvAdj!Q27:Q28)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH8ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH8ConvAdj_Quote#0003</v>
       </c>
       <c r="AI28" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH28)</f>
@@ -39824,7 +39756,7 @@
       </c>
       <c r="AH29" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG29,IborIndex,AF29,F29,Volatility,MeanReversion,Permanent,AND(ISERROR(Z29),ISERROR(FuturesHWConvAdj!Q28:Q29)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM8ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM8ConvAdj_Quote#0003</v>
       </c>
       <c r="AI29" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH29)</f>
@@ -39921,7 +39853,7 @@
       </c>
       <c r="AH30" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG30,IborIndex,AF30,F30,Volatility,MeanReversion,Permanent,AND(ISERROR(Z30),ISERROR(FuturesHWConvAdj!Q29:Q30)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU8ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU8ConvAdj_Quote#0003</v>
       </c>
       <c r="AI30" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH30)</f>
@@ -40018,7 +39950,7 @@
       </c>
       <c r="AH31" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG31,IborIndex,AF31,F31,Volatility,MeanReversion,Permanent,AND(ISERROR(Z31),ISERROR(FuturesHWConvAdj!Q30:Q31)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ8ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ8ConvAdj_Quote#0003</v>
       </c>
       <c r="AI31" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH31)</f>
@@ -40115,7 +40047,7 @@
       </c>
       <c r="AH32" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG32,IborIndex,AF32,F32,Volatility,MeanReversion,Permanent,AND(ISERROR(Z32),ISERROR(FuturesHWConvAdj!Q31:Q32)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH9ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH9ConvAdj_Quote#0003</v>
       </c>
       <c r="AI32" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH32)</f>
@@ -40212,7 +40144,7 @@
       </c>
       <c r="AH33" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG33,IborIndex,AF33,F33,Volatility,MeanReversion,Permanent,AND(ISERROR(Z33),ISERROR(FuturesHWConvAdj!Q32:Q33)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM9ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM9ConvAdj_Quote#0003</v>
       </c>
       <c r="AI33" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH33)</f>
@@ -40309,7 +40241,7 @@
       </c>
       <c r="AH34" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG34,IborIndex,AF34,F34,Volatility,MeanReversion,Permanent,AND(ISERROR(Z34),ISERROR(FuturesHWConvAdj!Q33:Q34)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU9ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU9ConvAdj_Quote#0003</v>
       </c>
       <c r="AI34" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH34)</f>
@@ -40406,7 +40338,7 @@
       </c>
       <c r="AH35" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG35,IborIndex,AF35,F35,Volatility,MeanReversion,Permanent,AND(ISERROR(Z35),ISERROR(FuturesHWConvAdj!Q34:Q35)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ9ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ9ConvAdj_Quote#0003</v>
       </c>
       <c r="AI35" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH35)</f>
@@ -40503,7 +40435,7 @@
       </c>
       <c r="AH36" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG36,IborIndex,AF36,F36,Volatility,MeanReversion,Permanent,AND(ISERROR(Z36),ISERROR(FuturesHWConvAdj!Q35:Q36)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH0ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH0ConvAdj_Quote#0003</v>
       </c>
       <c r="AI36" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH36)</f>
@@ -40600,7 +40532,7 @@
       </c>
       <c r="AH37" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG37,IborIndex,AF37,F37,Volatility,MeanReversion,Permanent,AND(ISERROR(Z37),ISERROR(FuturesHWConvAdj!Q36:Q37)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM0ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM0ConvAdj_Quote#0003</v>
       </c>
       <c r="AI37" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH37)</f>
@@ -40697,7 +40629,7 @@
       </c>
       <c r="AH38" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG38,IborIndex,AF38,F38,Volatility,MeanReversion,Permanent,AND(ISERROR(Z38),ISERROR(FuturesHWConvAdj!Q37:Q38)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU0ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU0ConvAdj_Quote#0003</v>
       </c>
       <c r="AI38" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH38)</f>
@@ -40794,7 +40726,7 @@
       </c>
       <c r="AH39" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG39,IborIndex,AF39,F39,Volatility,MeanReversion,Permanent,AND(ISERROR(Z39),ISERROR(FuturesHWConvAdj!Q38:Q39)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ0ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ0ConvAdj_Quote#0003</v>
       </c>
       <c r="AI39" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH39)</f>
@@ -40891,7 +40823,7 @@
       </c>
       <c r="AH40" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG40,IborIndex,AF40,F40,Volatility,MeanReversion,Permanent,AND(ISERROR(Z40),ISERROR(FuturesHWConvAdj!Q39:Q40)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH1ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH1ConvAdj_Quote#0003</v>
       </c>
       <c r="AI40" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH40)</f>
@@ -40988,7 +40920,7 @@
       </c>
       <c r="AH41" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG41,IborIndex,AF41,F41,Volatility,MeanReversion,Permanent,AND(ISERROR(Z41),ISERROR(FuturesHWConvAdj!Q40:Q41)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM1ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM1ConvAdj_Quote#0003</v>
       </c>
       <c r="AI41" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH41)</f>
@@ -41085,7 +41017,7 @@
       </c>
       <c r="AH42" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG42,IborIndex,AF42,F42,Volatility,MeanReversion,Permanent,AND(ISERROR(Z42),ISERROR(FuturesHWConvAdj!Q41:Q42)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU1ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU1ConvAdj_Quote#0003</v>
       </c>
       <c r="AI42" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH42)</f>
@@ -41182,7 +41114,7 @@
       </c>
       <c r="AH43" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG43,IborIndex,AF43,F43,Volatility,MeanReversion,Permanent,AND(ISERROR(Z43),ISERROR(FuturesHWConvAdj!Q42:Q43)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ1ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ1ConvAdj_Quote#0003</v>
       </c>
       <c r="AI43" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH43)</f>
@@ -41279,7 +41211,7 @@
       </c>
       <c r="AH44" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG44,IborIndex,AF44,F44,Volatility,MeanReversion,Permanent,AND(ISERROR(Z44),ISERROR(FuturesHWConvAdj!Q43:Q44)),ObjectOverwrite)</f>
-        <v>AUDFUT3MH2ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MH2ConvAdj_Quote#0003</v>
       </c>
       <c r="AI44" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH44)</f>
@@ -41376,7 +41308,7 @@
       </c>
       <c r="AH45" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG45,IborIndex,AF45,F45,Volatility,MeanReversion,Permanent,AND(ISERROR(Z45),ISERROR(FuturesHWConvAdj!Q44:Q45)),ObjectOverwrite)</f>
-        <v>AUDFUT3MM2ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MM2ConvAdj_Quote#0003</v>
       </c>
       <c r="AI45" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH45)</f>
@@ -41473,7 +41405,7 @@
       </c>
       <c r="AH46" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG46,IborIndex,AF46,F46,Volatility,MeanReversion,Permanent,AND(ISERROR(Z46),ISERROR(FuturesHWConvAdj!Q45:Q46)),ObjectOverwrite)</f>
-        <v>AUDFUT3MU2ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MU2ConvAdj_Quote#0003</v>
       </c>
       <c r="AI46" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH46)</f>
@@ -41570,7 +41502,7 @@
       </c>
       <c r="AH47" s="129" t="str">
         <f>_xll.qlFuturesConvAdjustmentQuote(AG47,IborIndex,AF47,F47,Volatility,MeanReversion,Permanent,AND(ISERROR(Z47),ISERROR(FuturesHWConvAdj!Q46:Q47)),ObjectOverwrite)</f>
-        <v>AUDFUT3MZ2ConvAdj_Quote#0006</v>
+        <v>AUDFUT3MZ2ConvAdj_Quote#0003</v>
       </c>
       <c r="AI47" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(AH47)</f>

</xml_diff>